<commit_message>
data anaysis for 4/20 test
</commit_message>
<xml_diff>
--- a/Experimentation and Data Analysis/4-19TestData/DOE_results.xlsx
+++ b/Experimentation and Data Analysis/4-19TestData/DOE_results.xlsx
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t xml:space="preserve">toast </t>
   </si>
@@ -282,6 +282,15 @@
   </si>
   <si>
     <t>sid</t>
+  </si>
+  <si>
+    <t>Cook Time&amp; Delay</t>
+  </si>
+  <si>
+    <t>Bi</t>
+  </si>
+  <si>
+    <t>Bij</t>
   </si>
 </sst>
 </file>
@@ -389,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -399,6 +408,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1035,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD20"/>
+  <dimension ref="A1:AD22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1290,11 +1302,11 @@
         <v>-1</v>
       </c>
       <c r="V9" t="e">
-        <f>AVERAGE(N9,U9)</f>
+        <f t="shared" ref="V9:V16" si="0">AVERAGE(N9,U9)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W9" t="e">
-        <f>((N9-V9)^2+(U9-V9)^2)/(2-1)</f>
+        <f t="shared" ref="W9:W16" si="1">((N9-V9)^2+(U9-V9)^2)/(2-1)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="X9" t="e">
@@ -1302,7 +1314,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Y9" t="e">
-        <f>AVERAGE(L9,S9)</f>
+        <f t="shared" ref="Y9:Y16" si="2">AVERAGE(L9,S9)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Z9" t="e">
@@ -1340,43 +1352,43 @@
         <v>-1</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10:F16" si="0">C10*D10*E10</f>
+        <f t="shared" ref="F10:F16" si="3">C10*D10*E10</f>
         <v>1</v>
       </c>
       <c r="V10" t="e">
-        <f>AVERAGE(N10,U10)</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W10" t="e">
-        <f>((N10-V10)^2+(U10-V10)^2)/(2-1)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="X10" t="e">
-        <f t="shared" ref="X10:X16" si="1">SQRT(W10)</f>
+        <f t="shared" ref="X10:X16" si="4">SQRT(W10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Y10" t="e">
-        <f>AVERAGE(L10,S10)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z10" t="e">
-        <f t="shared" ref="Z10:Z16" si="2">((L10-Y10)^2+(S10-Y10)^2)/(2-1)</f>
+        <f t="shared" ref="Z10:Z16" si="5">((L10-Y10)^2+(S10-Y10)^2)/(2-1)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AA10" t="e">
-        <f t="shared" ref="AA10:AA16" si="3">SQRT(Z10)</f>
+        <f t="shared" ref="AA10:AA16" si="6">SQRT(Z10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AB10" t="e">
-        <f t="shared" ref="AB10:AB16" si="4">AVERAGE(M10,T10)</f>
+        <f t="shared" ref="AB10:AB16" si="7">AVERAGE(M10,T10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AC10" t="e">
-        <f t="shared" ref="AC10:AC16" si="5">((M10-AB10)^2+(T10-AB10)^2)/(2-1)</f>
+        <f t="shared" ref="AC10:AC16" si="8">((M10-AB10)^2+(T10-AB10)^2)/(2-1)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AD10" t="e">
-        <f t="shared" ref="AD10:AD16" si="6">SQRT(AC10)</f>
+        <f t="shared" ref="AD10:AD16" si="9">SQRT(AC10)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1397,7 +1409,7 @@
         <v>-1</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G11">
@@ -1420,39 +1432,39 @@
         <v>541.125</v>
       </c>
       <c r="V11">
-        <f>AVERAGE(N11,U11)</f>
+        <f t="shared" si="0"/>
         <v>541.125</v>
       </c>
       <c r="W11">
-        <f>((N11-V11)^2+(U11-V11)^2)/(2-1)</f>
+        <f t="shared" si="1"/>
         <v>292816.265625</v>
       </c>
       <c r="X11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>541.125</v>
       </c>
       <c r="Y11">
-        <f>AVERAGE(L11,S11)</f>
+        <f t="shared" si="2"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>7.8400000000000011E-2</v>
       </c>
       <c r="AA11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="AB11" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC11" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD11" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1470,43 +1482,43 @@
         <v>-1</v>
       </c>
       <c r="F12">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="V12" t="e">
         <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="V12" t="e">
-        <f>AVERAGE(N12,U12)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W12" t="e">
-        <f>((N12-V12)^2+(U12-V12)^2)/(2-1)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="X12" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y12" t="e">
-        <f>AVERAGE(L12,S12)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z12" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA12" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB12" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC12" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD12" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1527,7 +1539,7 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G13">
@@ -1550,39 +1562,39 @@
         <v>400.90100000000001</v>
       </c>
       <c r="V13">
-        <f>AVERAGE(N13,U13)</f>
+        <f t="shared" si="0"/>
         <v>400.90100000000001</v>
       </c>
       <c r="W13">
-        <f>((N13-V13)^2+(U13-V13)^2)/(2-1)</f>
+        <f t="shared" si="1"/>
         <v>160721.61180100002</v>
       </c>
       <c r="X13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>400.90100000000001</v>
       </c>
       <c r="Y13">
-        <f>AVERAGE(L13,S13)</f>
+        <f t="shared" si="2"/>
         <v>0.27</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>7.2900000000000006E-2</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.27</v>
       </c>
       <c r="AB13" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC13" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD13" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1603,7 +1615,7 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
       <c r="G14">
@@ -1625,39 +1637,39 @@
         <v>424.09500000000003</v>
       </c>
       <c r="V14">
-        <f>AVERAGE(N14,U14)</f>
+        <f t="shared" si="0"/>
         <v>424.09500000000003</v>
       </c>
       <c r="W14">
-        <f>((N14-V14)^2+(U14-V14)^2)/(2-1)</f>
+        <f t="shared" si="1"/>
         <v>179856.56902500003</v>
       </c>
       <c r="X14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>424.09500000000003</v>
       </c>
       <c r="Y14">
-        <f>AVERAGE(L14,S14)</f>
+        <f t="shared" si="2"/>
         <v>0.27</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>7.2900000000000006E-2</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.27</v>
       </c>
       <c r="AB14" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC14" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD14" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1678,7 +1690,7 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
       <c r="G15">
@@ -1700,39 +1712,39 @@
         <v>523.80499999999995</v>
       </c>
       <c r="V15">
-        <f>AVERAGE(N15,U15)</f>
+        <f t="shared" si="0"/>
         <v>523.80499999999995</v>
       </c>
       <c r="W15">
-        <f>((N15-V15)^2+(U15-V15)^2)/(2-1)</f>
+        <f t="shared" si="1"/>
         <v>274371.67802499997</v>
       </c>
       <c r="X15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>523.80499999999995</v>
       </c>
       <c r="Y15">
-        <f>AVERAGE(L15,S15)</f>
+        <f t="shared" si="2"/>
         <v>0.26</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.7600000000000007E-2</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.26</v>
       </c>
       <c r="AB15" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC15" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1753,7 +1765,7 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G16">
@@ -1776,43 +1788,49 @@
         <v>421.73099999999999</v>
       </c>
       <c r="V16">
-        <f>AVERAGE(N16,U16)</f>
+        <f t="shared" si="0"/>
         <v>421.73099999999999</v>
       </c>
       <c r="W16">
-        <f>((N16-V16)^2+(U16-V16)^2)/(2-1)</f>
+        <f t="shared" si="1"/>
         <v>177857.03636100001</v>
       </c>
       <c r="X16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>421.73099999999999</v>
       </c>
       <c r="Y16">
-        <f>AVERAGE(L16,S16)</f>
+        <f t="shared" si="2"/>
         <v>0.27</v>
       </c>
       <c r="Z16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>7.2900000000000006E-2</v>
       </c>
       <c r="AA16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.27</v>
       </c>
       <c r="AB16" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC16" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD16" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+    </row>
     <row r="18" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
         <v>32</v>
@@ -1844,8 +1862,25 @@
       <c r="B20" t="s">
         <v>35</v>
       </c>
+      <c r="C20">
+        <f>AVERAGE(N10,N11,N13,N16,U10,U11,U13,U16)-AVERAGE(N9,N12,N14:N15,U9,U12,U14:U15)</f>
+        <v>-19.36433333333332</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A17:C17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Continued to process experimental data
</commit_message>
<xml_diff>
--- a/Experimentation and Data Analysis/4-19TestData/DOE_results.xlsx
+++ b/Experimentation and Data Analysis/4-19TestData/DOE_results.xlsx
@@ -29,6 +29,80 @@
     <author>Claire Puccini</author>
   </authors>
   <commentList>
+    <comment ref="B9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Claire Puccini:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+two proximity delay, 
+more eggy </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Claire Puccini:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+no eccentric movement of motor
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Claire Puccini:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+more eggy than yesterdays test </t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B11" authorId="0" shapeId="0">
       <text>
         <r>
@@ -55,6 +129,78 @@
         </r>
       </text>
     </comment>
+    <comment ref="Q11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Claire Puccini:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+serial monitor not opened, delayed placement on stove for 30s, watery </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Claire Puccini:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+issue opening serial monitor, may have led to additional time spent on stove sitting w/ stirring, one side still higher than the other, powder sat in a small amount of water so it clumped, more eggy</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Claire Puccini:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+"this actually looks appetizing" -Sid</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B14" authorId="0" shapeId="0">
       <text>
         <r>
@@ -76,6 +222,30 @@
           </rPr>
           <t xml:space="preserve">
 measured jar after blended, some powder left on blender, 2 random delay?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Claire Puccini:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+coupling set screw came loose </t>
         </r>
       </text>
     </comment>
@@ -109,7 +279,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="57">
   <si>
     <t xml:space="preserve">toast </t>
   </si>
@@ -139,36 +309,6 @@
   </si>
   <si>
     <t>Propeller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cold </t>
-  </si>
-  <si>
-    <t>key</t>
-  </si>
-  <si>
-    <t>water:</t>
-  </si>
-  <si>
-    <t>stirring pattern:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">propeller type </t>
-  </si>
-  <si>
-    <t>w/ delay</t>
-  </si>
-  <si>
-    <t>no delay</t>
-  </si>
-  <si>
-    <t>room</t>
-  </si>
-  <si>
-    <t>curved w/ slit</t>
-  </si>
-  <si>
-    <t>flat w/o slit</t>
   </si>
   <si>
     <r>
@@ -190,9 +330,6 @@
     <t xml:space="preserve">Egg Weight </t>
   </si>
   <si>
-    <t>Water Loss</t>
-  </si>
-  <si>
     <t>Consistency</t>
   </si>
   <si>
@@ -260,9 +397,6 @@
     <t>Egg Weight (g)</t>
   </si>
   <si>
-    <t>Water Loss (g)</t>
-  </si>
-  <si>
     <t xml:space="preserve">tupperware </t>
   </si>
   <si>
@@ -284,20 +418,71 @@
     <t>sid</t>
   </si>
   <si>
-    <t>Cook Time&amp; Delay</t>
-  </si>
-  <si>
     <t>Bi</t>
   </si>
   <si>
     <t>Bij</t>
+  </si>
+  <si>
+    <t>Cold water</t>
+  </si>
+  <si>
+    <t>cold water</t>
+  </si>
+  <si>
+    <t>propeller</t>
+  </si>
+  <si>
+    <t>full jar (g)</t>
+  </si>
+  <si>
+    <t>toast</t>
+  </si>
+  <si>
+    <t>tupperware weight (g)</t>
+  </si>
+  <si>
+    <t>start time</t>
+  </si>
+  <si>
+    <t>Material Loss (g)</t>
+  </si>
+  <si>
+    <t>Cold Water</t>
+  </si>
+  <si>
+    <t>Average Temp</t>
+  </si>
+  <si>
+    <t>Material Loss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">equations </t>
+  </si>
+  <si>
+    <t>Cook time:</t>
+  </si>
+  <si>
+    <t>Average Temp:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Material Loss: </t>
+  </si>
+  <si>
+    <t>y=448+7.93x1+-15.41x2+-38.98x3+-19.52x123</t>
+  </si>
+  <si>
+    <t>y=63.64+0.60x1+0.67x2+-0.11x3+1.03x123</t>
+  </si>
+  <si>
+    <t>y=69+-0.38x1+-2.38x2+2.50x3+-3.25x123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,6 +531,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -398,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -408,9 +606,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,16 +642,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>23813</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>319089</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>138111</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>42863</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>128588</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>223838</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>-1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -455,8 +660,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2890838" y="4005263"/>
-          <a:ext cx="2571750" cy="1595438"/>
+          <a:off x="10034589" y="3257549"/>
+          <a:ext cx="2457449" cy="2576513"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -534,7 +739,12 @@
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t>-plan pan correctly </a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>-soldered the connection points in the blender and motor, between 4/20 and 4/21 </a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -542,16 +752,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4763</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>347663</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>138113</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -560,8 +770,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4763" y="4005263"/>
-          <a:ext cx="2571750" cy="2652712"/>
+          <a:off x="6867525" y="3238500"/>
+          <a:ext cx="2986088" cy="2857500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -649,7 +859,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>-periodic delay </a:t>
+            <a:t>-periodic delay 2s</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -661,7 +871,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>-backward spin 2s</a:t>
+            <a:t>-backward spin 3s</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -690,16 +900,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>400051</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>138113</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>419101</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>104776</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -708,8 +918,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5819776" y="3981451"/>
-          <a:ext cx="2571750" cy="1595438"/>
+          <a:off x="12611100" y="3262312"/>
+          <a:ext cx="3209925" cy="2143125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -774,6 +984,105 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t>-inconsistent propeller scrapping </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>-after trial 5 of the second run (6,7,8) the scale was run from a 9 v  power supply </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>-should have measured after blending and the propeller was removed </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>14290</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>200027</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6862765" y="6157914"/>
+          <a:ext cx="3052762" cy="1095374"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Key:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>-</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Stirring pattern: w/ delay 1     no delay -1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>-water: 	  room 1	cold -1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>-propeller	curved w/slit 1	flat w/o slit -1</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -1047,28 +1356,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD22"/>
+  <dimension ref="A1:AH45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="13.15625" bestFit="1" customWidth="1"/>
-    <col min="7" max="13" width="8.83984375" customWidth="1"/>
-    <col min="15" max="20" width="8.83984375" customWidth="1"/>
+    <col min="2" max="2" width="4.89453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.15625" customWidth="1"/>
+    <col min="4" max="4" width="4.578125" customWidth="1"/>
+    <col min="5" max="5" width="5" customWidth="1"/>
+    <col min="6" max="6" width="6.41796875" customWidth="1"/>
+    <col min="7" max="7" width="5.47265625" customWidth="1"/>
+    <col min="8" max="14" width="8.83984375" customWidth="1"/>
+    <col min="16" max="16" width="13.15625" bestFit="1" customWidth="1"/>
+    <col min="17" max="24" width="8.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1078,23 +1391,8 @@
       <c r="C2">
         <v>25</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1104,23 +1402,8 @@
       <c r="C3">
         <v>26</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1130,23 +1413,8 @@
       <c r="C4">
         <v>77</v>
       </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1157,9 +1425,9 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="H7" s="8" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -1167,34 +1435,38 @@
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
-      <c r="O7" s="7" t="s">
-        <v>27</v>
-      </c>
+      <c r="O7" s="8"/>
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
+      <c r="R7" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
-      <c r="V7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z7" s="5"/>
-      <c r="AA7" s="5"/>
-      <c r="AB7" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC7" s="6"/>
-      <c r="AD7" s="6"/>
-    </row>
-    <row r="8" spans="1:30" ht="17.7" x14ac:dyDescent="0.75">
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG7" s="6"/>
+      <c r="AH7" s="6"/>
+    </row>
+    <row r="8" spans="1:34" ht="17.7" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -1209,82 +1481,97 @@
         <v>9</v>
       </c>
       <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>42</v>
+      </c>
+      <c r="R8" t="s">
+        <v>14</v>
+      </c>
+      <c r="S8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T8" t="s">
+        <v>44</v>
+      </c>
+      <c r="U8" t="s">
+        <v>11</v>
+      </c>
+      <c r="V8" t="s">
+        <v>49</v>
+      </c>
+      <c r="W8" t="s">
+        <v>12</v>
+      </c>
+      <c r="X8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA8" t="s">
         <v>20</v>
       </c>
-      <c r="G8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" t="s">
-        <v>41</v>
-      </c>
-      <c r="L8" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" t="s">
-        <v>46</v>
-      </c>
-      <c r="N8" t="s">
-        <v>37</v>
-      </c>
-      <c r="O8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>21</v>
-      </c>
-      <c r="R8" t="s">
-        <v>22</v>
-      </c>
-      <c r="S8" t="s">
-        <v>23</v>
-      </c>
-      <c r="T8" t="s">
-        <v>47</v>
-      </c>
-      <c r="U8" t="s">
-        <v>24</v>
-      </c>
-      <c r="V8" t="s">
-        <v>29</v>
-      </c>
-      <c r="W8" t="s">
-        <v>31</v>
-      </c>
-      <c r="X8" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>30</v>
-      </c>
       <c r="AB8" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="AC8" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="AD8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+        <v>20</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="9">
+        <v>43211.081944444442</v>
+      </c>
       <c r="B9">
         <v>1</v>
       </c>
@@ -1301,44 +1588,108 @@
         <f>C9*D9*E9</f>
         <v>-1</v>
       </c>
-      <c r="V9" t="e">
-        <f t="shared" ref="V9:V16" si="0">AVERAGE(N9,U9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W9" t="e">
-        <f t="shared" ref="W9:W16" si="1">((N9-V9)^2+(U9-V9)^2)/(2-1)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X9" t="e">
-        <f>SQRT(W9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y9" t="e">
-        <f t="shared" ref="Y9:Y16" si="2">AVERAGE(L9,S9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Z9" t="e">
-        <f>((L9-Y9)^2+(S9-Y9)^2)/(2-1)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA9" t="e">
-        <f>SQRT(Z9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB9" t="e">
-        <f>AVERAGE(M9,T9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC9" t="e">
-        <f>((M9-AB9)^2+(T9-AB9)^2)/(2-1)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AD9" t="e">
-        <f>SQRT(AC9)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+      <c r="G9">
+        <v>513</v>
+      </c>
+      <c r="H9">
+        <v>256</v>
+      </c>
+      <c r="I9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9">
+        <v>77</v>
+      </c>
+      <c r="K9">
+        <v>247</v>
+      </c>
+      <c r="L9">
+        <f>(G9-H9)-(K9-J9)</f>
+        <v>87</v>
+      </c>
+      <c r="M9">
+        <v>0.27</v>
+      </c>
+      <c r="N9">
+        <v>66.39</v>
+      </c>
+      <c r="O9">
+        <f>(740730-121134)/1000</f>
+        <v>619.596</v>
+      </c>
+      <c r="P9" s="1">
+        <v>43202.181250000001</v>
+      </c>
+      <c r="Q9">
+        <v>512</v>
+      </c>
+      <c r="R9">
+        <v>268</v>
+      </c>
+      <c r="S9" t="s">
+        <v>43</v>
+      </c>
+      <c r="T9">
+        <v>25</v>
+      </c>
+      <c r="U9">
+        <v>210</v>
+      </c>
+      <c r="V9">
+        <f>(Q9-R9)-(U9-T9)</f>
+        <v>59</v>
+      </c>
+      <c r="W9">
+        <v>0.26</v>
+      </c>
+      <c r="X9">
+        <v>51.66</v>
+      </c>
+      <c r="Y9">
+        <f>(589783-143635)/1000</f>
+        <v>446.14800000000002</v>
+      </c>
+      <c r="Z9">
+        <f>AVERAGE(O9,Y9)</f>
+        <v>532.87200000000007</v>
+      </c>
+      <c r="AA9">
+        <f>((O9-Z9)^2+(Y9-Z9)^2)/(2-1)</f>
+        <v>15042.104351999997</v>
+      </c>
+      <c r="AB9">
+        <f>SQRT(AA9)</f>
+        <v>122.64625698324429</v>
+      </c>
+      <c r="AC9">
+        <f t="shared" ref="AC9:AC16" si="0">AVERAGE(M9,W9)</f>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="AD9">
+        <f>((M9-AC9)^2+(W9-AC9)^2)/(2-1)</f>
+        <v>5.000000000000009E-5</v>
+      </c>
+      <c r="AE9">
+        <f>SQRT(AD9)</f>
+        <v>7.0710678118654814E-3</v>
+      </c>
+      <c r="AF9">
+        <f>AVERAGE(N9,X9)</f>
+        <v>59.024999999999999</v>
+      </c>
+      <c r="AG9">
+        <f>((N9-AF9)^2+(X9-AF9)^2)/(2-1)</f>
+        <v>108.48645000000006</v>
+      </c>
+      <c r="AH9">
+        <f>SQRT(AG9)</f>
+        <v>10.415682886877848</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1">
+        <v>43211.094444444447</v>
+      </c>
       <c r="B10">
         <v>2</v>
       </c>
@@ -1352,47 +1703,109 @@
         <v>-1</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10:F16" si="3">C10*D10*E10</f>
+        <f t="shared" ref="F10:F16" si="1">C10*D10*E10</f>
         <v>1</v>
       </c>
-      <c r="V10" t="e">
+      <c r="G10">
+        <v>521</v>
+      </c>
+      <c r="H10">
+        <v>261</v>
+      </c>
+      <c r="I10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>25</v>
+      </c>
+      <c r="K10">
+        <v>220</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ref="L10:L16" si="2">(G10-H10)-(K10-J10)</f>
+        <v>65</v>
+      </c>
+      <c r="M10">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="N10">
+        <v>66.67</v>
+      </c>
+      <c r="O10">
+        <f>(595490-168671)/1000</f>
+        <v>426.81900000000002</v>
+      </c>
+      <c r="P10" s="1">
+        <v>43211.166666666664</v>
+      </c>
+      <c r="Q10">
+        <v>516</v>
+      </c>
+      <c r="R10">
+        <v>271</v>
+      </c>
+      <c r="S10" t="s">
+        <v>43</v>
+      </c>
+      <c r="T10">
+        <v>25</v>
+      </c>
+      <c r="U10">
+        <v>213</v>
+      </c>
+      <c r="V10">
+        <f t="shared" ref="V10:V16" si="3">(Q10-R10)-(U10-T10)</f>
+        <v>57</v>
+      </c>
+      <c r="W10">
+        <f>0.27</f>
+        <v>0.27</v>
+      </c>
+      <c r="X10">
+        <v>67.73</v>
+      </c>
+      <c r="Y10">
+        <f>(1157316-619644)/1000</f>
+        <v>537.67200000000003</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" ref="Z10:Z16" si="4">AVERAGE(O10,Y10)</f>
+        <v>482.24549999999999</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" ref="AA10:AA16" si="5">((O10-Z10)^2+(Y10-Z10)^2)/(2-1)</f>
+        <v>6144.1938045000006</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" ref="AB10:AB16" si="6">SQRT(AA10)</f>
+        <v>78.384908014872352</v>
+      </c>
+      <c r="AC10">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X10" t="e">
-        <f t="shared" ref="X10:X16" si="4">SQRT(W10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y10" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Z10" t="e">
-        <f t="shared" ref="Z10:Z16" si="5">((L10-Y10)^2+(S10-Y10)^2)/(2-1)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA10" t="e">
-        <f t="shared" ref="AA10:AA16" si="6">SQRT(Z10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB10" t="e">
-        <f t="shared" ref="AB10:AB16" si="7">AVERAGE(M10,T10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC10" t="e">
-        <f t="shared" ref="AC10:AC16" si="8">((M10-AB10)^2+(T10-AB10)^2)/(2-1)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AD10" t="e">
-        <f t="shared" ref="AD10:AD16" si="9">SQRT(AC10)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" ref="AD10:AD16" si="7">((M10-AC10)^2+(W10-AC10)^2)/(2-1)</f>
+        <v>5.000000000000009E-5</v>
+      </c>
+      <c r="AE10">
+        <f t="shared" ref="AE10:AE16" si="8">SQRT(AD10)</f>
+        <v>7.0710678118654814E-3</v>
+      </c>
+      <c r="AF10">
+        <f t="shared" ref="AF10:AF16" si="9">AVERAGE(N10,X10)</f>
+        <v>67.2</v>
+      </c>
+      <c r="AG10">
+        <f t="shared" ref="AG10:AG16" si="10">((N10-AF10)^2+(X10-AF10)^2)/(2-1)</f>
+        <v>0.56180000000000241</v>
+      </c>
+      <c r="AH10">
+        <f t="shared" ref="AH10:AH16" si="11">SQRT(AG10)</f>
+        <v>0.74953318805774194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>43210.19027777778</v>
       </c>
@@ -1409,7 +1822,7 @@
         <v>-1</v>
       </c>
       <c r="F11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G11">
@@ -1422,53 +1835,95 @@
         <v>0</v>
       </c>
       <c r="J11">
+        <v>25</v>
+      </c>
+      <c r="K11">
         <v>222</v>
       </c>
       <c r="L11">
+        <f t="shared" si="2"/>
+        <v>73</v>
+      </c>
+      <c r="M11">
         <v>0.28000000000000003</v>
       </c>
       <c r="N11">
+        <v>59.375</v>
+      </c>
+      <c r="O11">
         <f>(695760-154635)/1000</f>
         <v>541.125</v>
       </c>
+      <c r="Q11">
+        <v>508</v>
+      </c>
+      <c r="R11">
+        <v>246</v>
+      </c>
+      <c r="S11" t="s">
+        <v>43</v>
+      </c>
+      <c r="T11">
+        <v>25</v>
+      </c>
+      <c r="U11">
+        <v>233</v>
+      </c>
       <c r="V11">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+      <c r="W11">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="X11">
+        <v>70.266999999999996</v>
+      </c>
+      <c r="Y11">
+        <f>(431110-54132)/1000</f>
+        <v>376.97800000000001</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="4"/>
+        <v>459.05150000000003</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" si="5"/>
+        <v>13472.118804499998</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" si="6"/>
+        <v>116.06945681142821</v>
+      </c>
+      <c r="AC11">
         <f t="shared" si="0"/>
-        <v>541.125</v>
-      </c>
-      <c r="W11">
-        <f t="shared" si="1"/>
-        <v>292816.265625</v>
-      </c>
-      <c r="X11">
-        <f t="shared" si="4"/>
-        <v>541.125</v>
-      </c>
-      <c r="Y11">
-        <f t="shared" si="2"/>
         <v>0.28000000000000003</v>
       </c>
-      <c r="Z11">
-        <f t="shared" si="5"/>
-        <v>7.8400000000000011E-2</v>
-      </c>
-      <c r="AA11">
-        <f t="shared" si="6"/>
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="AB11" t="e">
+      <c r="AD11">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC11" t="e">
+        <v>0</v>
+      </c>
+      <c r="AE11">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AD11" t="e">
+        <v>0</v>
+      </c>
+      <c r="AF11">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+        <v>64.820999999999998</v>
+      </c>
+      <c r="AG11">
+        <f t="shared" si="10"/>
+        <v>59.317831999999953</v>
+      </c>
+      <c r="AH11">
+        <f t="shared" si="11"/>
+        <v>7.7018070606838727</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1">
+        <v>43211.058333333334</v>
+      </c>
       <c r="B12">
         <v>4</v>
       </c>
@@ -1482,47 +1937,108 @@
         <v>-1</v>
       </c>
       <c r="F12">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="G12">
+        <v>510</v>
+      </c>
+      <c r="H12">
+        <v>250</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>26</v>
+      </c>
+      <c r="K12">
+        <v>215</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>71</v>
+      </c>
+      <c r="M12">
+        <v>0.27</v>
+      </c>
+      <c r="N12">
+        <v>63.875</v>
+      </c>
+      <c r="O12">
+        <f>(455924-46133)/1000</f>
+        <v>409.791</v>
+      </c>
+      <c r="P12" s="1">
+        <v>43211.15625</v>
+      </c>
+      <c r="Q12">
+        <v>506</v>
+      </c>
+      <c r="R12">
+        <v>252</v>
+      </c>
+      <c r="S12" t="s">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>26</v>
+      </c>
+      <c r="U12">
+        <v>214</v>
+      </c>
+      <c r="V12">
         <f t="shared" si="3"/>
-        <v>-1</v>
-      </c>
-      <c r="V12" t="e">
+        <v>66</v>
+      </c>
+      <c r="W12">
+        <v>0.27</v>
+      </c>
+      <c r="X12">
+        <v>64.015600000000006</v>
+      </c>
+      <c r="Y12">
+        <f>(1157316-619644)/1000</f>
+        <v>537.67200000000003</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="4"/>
+        <v>473.73149999999998</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="5"/>
+        <v>8176.7750805000032</v>
+      </c>
+      <c r="AB12">
+        <f t="shared" si="6"/>
+        <v>90.425522284916909</v>
+      </c>
+      <c r="AC12">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W12" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X12" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y12" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Z12" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA12" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB12" t="e">
+        <v>0.27</v>
+      </c>
+      <c r="AD12">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC12" t="e">
+        <v>0</v>
+      </c>
+      <c r="AE12">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AD12" t="e">
+        <v>0</v>
+      </c>
+      <c r="AF12">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+        <v>63.945300000000003</v>
+      </c>
+      <c r="AG12">
+        <f t="shared" si="10"/>
+        <v>9.8841800000008823E-3</v>
+      </c>
+      <c r="AH12">
+        <f t="shared" si="11"/>
+        <v>9.9419213434833023E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>43210.169444444444</v>
       </c>
@@ -1539,7 +2055,7 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G13">
@@ -1552,53 +2068,95 @@
         <v>0</v>
       </c>
       <c r="J13">
+        <v>25</v>
+      </c>
+      <c r="K13">
         <v>210</v>
       </c>
       <c r="L13">
+        <f t="shared" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="M13">
         <v>0.27</v>
       </c>
       <c r="N13">
+        <v>63.5625</v>
+      </c>
+      <c r="O13">
         <f>(668955-268054)/1000</f>
         <v>400.90100000000001</v>
       </c>
+      <c r="P13" s="1">
+        <v>43211.208333333336</v>
+      </c>
+      <c r="Q13">
+        <v>498</v>
+      </c>
+      <c r="R13">
+        <v>273</v>
+      </c>
+      <c r="S13" t="s">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>26</v>
+      </c>
+      <c r="U13">
+        <v>182</v>
+      </c>
       <c r="V13">
+        <f t="shared" si="3"/>
+        <v>69</v>
+      </c>
+      <c r="W13">
+        <v>0.27</v>
+      </c>
+      <c r="X13">
+        <v>62.92</v>
+      </c>
+      <c r="Y13">
+        <f>(468113-125634)/1000</f>
+        <v>342.47899999999998</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="4"/>
+        <v>371.69</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" si="5"/>
+        <v>1706.5650420000015</v>
+      </c>
+      <c r="AB13">
+        <f t="shared" si="6"/>
+        <v>41.310592370480499</v>
+      </c>
+      <c r="AC13">
         <f t="shared" si="0"/>
-        <v>400.90100000000001</v>
-      </c>
-      <c r="W13">
-        <f t="shared" si="1"/>
-        <v>160721.61180100002</v>
-      </c>
-      <c r="X13">
-        <f t="shared" si="4"/>
-        <v>400.90100000000001</v>
-      </c>
-      <c r="Y13">
-        <f t="shared" si="2"/>
         <v>0.27</v>
       </c>
-      <c r="Z13">
-        <f t="shared" si="5"/>
-        <v>7.2900000000000006E-2</v>
-      </c>
-      <c r="AA13">
-        <f t="shared" si="6"/>
-        <v>0.27</v>
-      </c>
-      <c r="AB13" t="e">
+      <c r="AD13">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC13" t="e">
+        <v>0</v>
+      </c>
+      <c r="AE13">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AD13" t="e">
+        <v>0</v>
+      </c>
+      <c r="AF13">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+        <v>63.241250000000001</v>
+      </c>
+      <c r="AG13">
+        <f t="shared" si="10"/>
+        <v>0.20640312499999891</v>
+      </c>
+      <c r="AH13">
+        <f t="shared" si="11"/>
+        <v>0.45431610691235558</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>43210.15347222222</v>
       </c>
@@ -1615,7 +2173,7 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="G14">
@@ -1628,52 +2186,94 @@
         <v>1</v>
       </c>
       <c r="J14">
+        <v>26</v>
+      </c>
+      <c r="K14">
         <v>223</v>
       </c>
       <c r="L14">
+        <f t="shared" si="2"/>
+        <v>74</v>
+      </c>
+      <c r="M14">
         <v>0.27</v>
       </c>
       <c r="N14">
+        <v>63.1875</v>
+      </c>
+      <c r="O14">
         <v>424.09500000000003</v>
       </c>
+      <c r="P14" s="1">
+        <v>43211.229166666664</v>
+      </c>
+      <c r="Q14">
+        <v>502</v>
+      </c>
+      <c r="R14">
+        <v>251</v>
+      </c>
+      <c r="S14" t="s">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>26</v>
+      </c>
+      <c r="U14">
+        <v>214</v>
+      </c>
       <c r="V14">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="W14">
+        <v>0.27</v>
+      </c>
+      <c r="X14">
+        <v>66.9375</v>
+      </c>
+      <c r="Y14">
+        <f>(1931393-1562166)/1000</f>
+        <v>369.22699999999998</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="4"/>
+        <v>396.661</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="5"/>
+        <v>1505.2487120000028</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" si="6"/>
+        <v>38.797534870143522</v>
+      </c>
+      <c r="AC14">
         <f t="shared" si="0"/>
-        <v>424.09500000000003</v>
-      </c>
-      <c r="W14">
-        <f t="shared" si="1"/>
-        <v>179856.56902500003</v>
-      </c>
-      <c r="X14">
-        <f t="shared" si="4"/>
-        <v>424.09500000000003</v>
-      </c>
-      <c r="Y14">
-        <f t="shared" si="2"/>
         <v>0.27</v>
       </c>
-      <c r="Z14">
-        <f t="shared" si="5"/>
-        <v>7.2900000000000006E-2</v>
-      </c>
-      <c r="AA14">
-        <f t="shared" si="6"/>
-        <v>0.27</v>
-      </c>
-      <c r="AB14" t="e">
+      <c r="AD14">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC14" t="e">
+        <v>0</v>
+      </c>
+      <c r="AE14">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AD14" t="e">
+        <v>0</v>
+      </c>
+      <c r="AF14">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+        <v>65.0625</v>
+      </c>
+      <c r="AG14">
+        <f t="shared" si="10"/>
+        <v>7.03125</v>
+      </c>
+      <c r="AH14">
+        <f t="shared" si="11"/>
+        <v>2.6516504294495533</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
         <v>43210.085416666669</v>
       </c>
@@ -1690,7 +2290,7 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="G15">
@@ -1703,52 +2303,94 @@
         <v>0</v>
       </c>
       <c r="J15">
+        <v>25</v>
+      </c>
+      <c r="K15">
         <v>168</v>
       </c>
       <c r="L15">
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
+      <c r="M15">
         <v>0.26</v>
       </c>
       <c r="N15">
+        <v>53.1875</v>
+      </c>
+      <c r="O15">
         <v>523.80499999999995</v>
       </c>
+      <c r="P15" s="1">
+        <v>43211.270833333336</v>
+      </c>
+      <c r="Q15">
+        <v>510</v>
+      </c>
+      <c r="R15">
+        <v>269</v>
+      </c>
+      <c r="S15" t="s">
+        <v>43</v>
+      </c>
+      <c r="T15">
+        <v>25</v>
+      </c>
+      <c r="U15">
+        <v>200</v>
+      </c>
       <c r="V15">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="W15">
+        <v>0.27</v>
+      </c>
+      <c r="X15">
+        <v>71.625</v>
+      </c>
+      <c r="Y15">
+        <f>(535961-126134)/1000</f>
+        <v>409.827</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="4"/>
+        <v>466.81599999999997</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" si="5"/>
+        <v>6495.4922419999948</v>
+      </c>
+      <c r="AB15">
+        <f t="shared" si="6"/>
+        <v>80.594616706080288</v>
+      </c>
+      <c r="AC15">
         <f t="shared" si="0"/>
-        <v>523.80499999999995</v>
-      </c>
-      <c r="W15">
-        <f t="shared" si="1"/>
-        <v>274371.67802499997</v>
-      </c>
-      <c r="X15">
-        <f t="shared" si="4"/>
-        <v>523.80499999999995</v>
-      </c>
-      <c r="Y15">
-        <f t="shared" si="2"/>
-        <v>0.26</v>
-      </c>
-      <c r="Z15">
-        <f t="shared" si="5"/>
-        <v>6.7600000000000007E-2</v>
-      </c>
-      <c r="AA15">
-        <f t="shared" si="6"/>
-        <v>0.26</v>
-      </c>
-      <c r="AB15" t="e">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="AD15">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC15" t="e">
+        <v>5.000000000000009E-5</v>
+      </c>
+      <c r="AE15">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AD15" t="e">
+        <v>7.0710678118654814E-3</v>
+      </c>
+      <c r="AF15">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.55000000000000004">
+        <v>62.40625</v>
+      </c>
+      <c r="AG15">
+        <f t="shared" si="10"/>
+        <v>169.970703125</v>
+      </c>
+      <c r="AH15">
+        <f t="shared" si="11"/>
+        <v>13.03728127812697</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3">
         <v>43210.151388888888</v>
       </c>
@@ -1765,7 +2407,7 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G16">
@@ -1775,111 +2417,716 @@
         <v>247</v>
       </c>
       <c r="I16" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="J16">
+        <v>77</v>
+      </c>
+      <c r="K16">
         <v>264</v>
       </c>
       <c r="L16">
+        <f t="shared" si="2"/>
+        <v>71</v>
+      </c>
+      <c r="M16">
         <v>0.27</v>
       </c>
       <c r="N16">
+        <v>64.75</v>
+      </c>
+      <c r="O16">
         <f>(559365-137634)/1000</f>
         <v>421.73099999999999</v>
       </c>
+      <c r="P16" s="1">
+        <v>43211.244444444441</v>
+      </c>
+      <c r="Q16">
+        <v>505</v>
+      </c>
+      <c r="R16">
+        <v>249</v>
+      </c>
+      <c r="S16" t="s">
+        <v>43</v>
+      </c>
+      <c r="T16">
+        <v>25</v>
+      </c>
+      <c r="U16">
+        <v>220</v>
+      </c>
       <c r="V16">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+      <c r="W16">
+        <v>0.27</v>
+      </c>
+      <c r="X16">
+        <v>62.09</v>
+      </c>
+      <c r="Y16">
+        <f>(814747-434640)/1000</f>
+        <v>380.10700000000003</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" si="4"/>
+        <v>400.91899999999998</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" si="5"/>
+        <v>866.27868799999862</v>
+      </c>
+      <c r="AB16">
+        <f t="shared" si="6"/>
+        <v>29.43261266010883</v>
+      </c>
+      <c r="AC16">
         <f t="shared" si="0"/>
-        <v>421.73099999999999</v>
-      </c>
-      <c r="W16">
-        <f t="shared" si="1"/>
-        <v>177857.03636100001</v>
-      </c>
-      <c r="X16">
-        <f t="shared" si="4"/>
-        <v>421.73099999999999</v>
-      </c>
-      <c r="Y16">
-        <f t="shared" si="2"/>
         <v>0.27</v>
       </c>
-      <c r="Z16">
-        <f t="shared" si="5"/>
-        <v>7.2900000000000006E-2</v>
-      </c>
-      <c r="AA16">
-        <f t="shared" si="6"/>
-        <v>0.27</v>
-      </c>
-      <c r="AB16" t="e">
+      <c r="AD16">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC16" t="e">
+        <v>0</v>
+      </c>
+      <c r="AE16">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AD16" t="e">
+        <v>0</v>
+      </c>
+      <c r="AF16">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="9" t="s">
+        <v>63.42</v>
+      </c>
+      <c r="AG16">
+        <f t="shared" si="10"/>
+        <v>3.537799999999991</v>
+      </c>
+      <c r="AH16">
+        <f t="shared" si="11"/>
+        <v>1.8809040379562141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+    </row>
+    <row r="19" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="13">
+        <f>AVERAGE(O9:O16,Y9:Y16)</f>
+        <v>447.99831250000005</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="2">
+        <f>AVERAGE(O9:O16,Y9:Y16)</f>
+        <v>447.99831250000005</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="13">
+        <f>AVERAGE(O9:O16,Y9:Y16)</f>
+        <v>447.99831250000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="13">
+        <f>AVERAGE(O10,O12,O15:O16,Y10,Y12,Y15:Y16)-AVERAGE(O9,O11,O13:O14,Y9,Y11,Y13:Y14)</f>
+        <v>15.859375</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="2">
+        <f>AVERAGE(O11,O12,O14,O16,Y11,Y12,Y14,Y16)-AVERAGE(O9,O10,O13,O15,Y9,Y10,Y13,Y15)</f>
+        <v>-30.81512500000008</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" s="13">
+        <f>AVERAGE(O13:O16,Y13:Y16)-AVERAGE(O9:O12,Y9:Y12)</f>
+        <v>-77.953625000000045</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="14">
+        <f>AVERAGE(O10,O11,O13,O16,Y10,Y11,Y13,Y16)-AVERAGE(O9,O12,O14:O15,Y9,Y12,Y14:Y15)</f>
+        <v>-39.04362500000002</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21">
+        <f>AVERAGE(O10,O11,O13,O16,Y10,Y11,Y13,Y16)-AVERAGE(O9,O12,O14,O15,Y9,Y12,Y14,Y15)</f>
+        <v>-39.04362500000002</v>
+      </c>
+      <c r="G21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" s="14">
+        <f>AVERAGE(O10,O11,O13,O16,Y10,Y11,Y13,Y16)-AVERAGE(O9,O12,O14,O15,Y9,Y12,Y14,Y15)</f>
+        <v>-39.04362500000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="14">
+        <f>C20/2</f>
+        <v>7.9296875</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22">
+        <f>F20/2</f>
+        <v>-15.40756250000004</v>
+      </c>
+      <c r="G22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I22" s="14">
+        <f>I20/2</f>
+        <v>-38.976812500000023</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="14">
+        <f>C21/2</f>
+        <v>-19.52181250000001</v>
+      </c>
+      <c r="D23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23">
+        <f>F21/2</f>
+        <v>-19.52181250000001</v>
+      </c>
+      <c r="G23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" t="s">
+        <v>41</v>
+      </c>
+      <c r="I23" s="14">
+        <f>I21/2</f>
+        <v>-19.52181250000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="13">
+        <f>AVERAGE(N9:N16,X9:X16)</f>
+        <v>63.640162500000002</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="13">
+        <f>AVERAGE(N9:N16,X9:X16)</f>
+        <v>63.640162500000002</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="13">
+        <f>AVERAGE(N9:N16,X9:X16)</f>
+        <v>63.640162500000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="13">
+        <f>AVERAGE(N10,N12,N15:N16,X10,X12,X15:X16)-AVERAGE(N9,N11,N13:N14,X9,X11,X13:X14)</f>
+        <v>1.2054500000000132</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="13">
+        <f>AVERAGE(N11:N12,N14,N16,X11:X12,X14,X16)-AVERAGE(N9:N10,N13,N15,X9:X10,X13,X15)</f>
+        <v>1.3440749999999966</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I27" s="13">
+        <f>AVERAGE(N13:N16,X13:X16)-AVERAGE(N9:N12,X9:X12)</f>
+        <v>-0.21532500000000709</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="14">
+        <f>AVERAGE(N10:N11,N13,N16,X10:X11,X13,X16)-AVERAGE(N9,N12,N14:N15,X9,X12,X14:X15)</f>
+        <v>2.0608000000000075</v>
+      </c>
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="14">
+        <f>AVERAGE(N10:N11,N13,N16,X10:X11,X13,X16)-AVERAGE(N9,N12,N14:N15,X9,X12,X14:X15)</f>
+        <v>2.0608000000000075</v>
+      </c>
+      <c r="G28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" t="s">
+        <v>41</v>
+      </c>
+      <c r="I28" s="14">
+        <f>AVERAGE(N10,N11,N13,N16,X10:X11,X13,X16)-AVERAGE(N9,N12,N14:N15,X9,X12,X14:X15)</f>
+        <v>2.0608000000000075</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="14">
+        <f>C27/2</f>
+        <v>0.60272500000000662</v>
+      </c>
+      <c r="D29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" s="14">
+        <f>F27/2</f>
+        <v>0.67203749999999829</v>
+      </c>
+      <c r="G29" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" t="s">
+        <v>41</v>
+      </c>
+      <c r="I29" s="14">
+        <f>I27/2</f>
+        <v>-0.10766250000000355</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="14">
+        <f>C28/2</f>
+        <v>1.0304000000000038</v>
+      </c>
+      <c r="D30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="14">
+        <f>F28/2</f>
+        <v>1.0304000000000038</v>
+      </c>
+      <c r="G30" t="s">
+        <v>38</v>
+      </c>
+      <c r="H30" t="s">
+        <v>41</v>
+      </c>
+      <c r="I30" s="14">
+        <f>I28/2</f>
+        <v>1.0304000000000038</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-    </row>
-    <row r="18" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="2">
-        <f>AVERAGE(N9:N16,U9:U16)</f>
-        <v>462.33140000000003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="2">
-        <f>AVERAGE(N10,N12,N15:N16,U10,U12,U15:U16)-AVERAGE(N9,N11,N13:N14,U9,U11,U13:U14)</f>
-        <v>17.394333333333293</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20">
-        <f>AVERAGE(N10,N11,N13,N16,U10,U11,U13,U16)-AVERAGE(N9,N12,N14:N15,U9,U12,U14:U15)</f>
-        <v>-19.36433333333332</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="13">
+        <f>AVERAGE(L9:L16,V9:V16)</f>
+        <v>69</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33" s="13">
+        <f>AVERAGE(L9:L16,V9:V16)</f>
+        <v>69</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" s="13">
+        <f>AVERAGE(L9:L16,V9:V16)</f>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="13">
+        <f>AVERAGE(L10,L12,L15:L16,V10,V12,V15:V16)-AVERAGE(L9,L11,L13:L14,V9,V11,V13:V14)</f>
+        <v>-0.75</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" s="13">
+        <f>AVERAGE(L11:L12,L14,L16,V11:V12,V14,V16)-AVERAGE(L9:L10,L13,L15,V9:V10,V13,V15)</f>
+        <v>-4.75</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I34" s="13">
+        <f>AVERAGE(L13:L16,V13:V16)-AVERAGE(L9:L12,V9:V12)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="13">
+        <f>AVERAGE(L10,L11,L13,L16,V10,V11,V13,V16)-AVERAGE(L9,L12,L14:L15,V9,V12,V14:V15)</f>
+        <v>-6.5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" s="14">
+        <f>AVERAGE(V10,V11,V13,V16,L10,L11,L13,L16)-AVERAGE(L9,L12,L14:L15,V9,V12,V14:V15)</f>
+        <v>-6.5</v>
+      </c>
+      <c r="G35" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" t="s">
+        <v>41</v>
+      </c>
+      <c r="I35" s="14">
+        <f>AVERAGE(L10:L11,L13,L16,V10:V11,V13,V16)-AVERAGE(L9,L12,L14:L15,V9,V12,V14:V15)</f>
+        <v>-6.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="14">
+        <f>C34/2</f>
+        <v>-0.375</v>
+      </c>
+      <c r="D36" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="14">
+        <f>F34/2</f>
+        <v>-2.375</v>
+      </c>
+      <c r="G36" t="s">
+        <v>37</v>
+      </c>
+      <c r="H36" t="s">
+        <v>41</v>
+      </c>
+      <c r="I36" s="14">
+        <f>I34/2</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="14">
+        <f>C35/2</f>
+        <v>-3.25</v>
+      </c>
+      <c r="D37" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" s="14">
+        <f>F35/2</f>
+        <v>-3.25</v>
+      </c>
+      <c r="G37" t="s">
+        <v>38</v>
+      </c>
+      <c r="H37" t="s">
+        <v>41</v>
+      </c>
+      <c r="I37" s="14">
+        <f>I35/2</f>
+        <v>-3.25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
         <v>51</v>
       </c>
     </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A17:C17"/>
+  <mergeCells count="12">
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A24:I24"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Recalculations for DOE and matlab code to plot
</commit_message>
<xml_diff>
--- a/Experimentation and Data Analysis/4-19TestData/DOE_results.xlsx
+++ b/Experimentation and Data Analysis/4-19TestData/DOE_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19176" windowHeight="6762" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19176" windowHeight="6762"/>
   </bookViews>
   <sheets>
     <sheet name="Unaltered Data" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q9" authorId="0" shapeId="0">
+    <comment ref="T9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -130,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q11" authorId="0" shapeId="0">
+    <comment ref="T11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -178,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q12" authorId="0" shapeId="0">
+    <comment ref="T12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -226,7 +226,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q14" authorId="0" shapeId="0">
+    <comment ref="T14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -535,7 +535,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="90">
   <si>
     <t xml:space="preserve">toast </t>
   </si>
@@ -744,6 +744,132 @@
   </si>
   <si>
     <t xml:space="preserve">Original Equations based off of unaltered data: </t>
+  </si>
+  <si>
+    <r>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>12</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>13</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>23</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Cook Time </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean response </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interaction </t>
+  </si>
+  <si>
+    <t>delay vs water</t>
+  </si>
+  <si>
+    <t>delay vs propeller</t>
+  </si>
+  <si>
+    <t>water vs propeller</t>
+  </si>
+  <si>
+    <t>Mean response</t>
+  </si>
+  <si>
+    <t>interaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean response </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final Temp </t>
+  </si>
+  <si>
+    <t>ME delay</t>
+  </si>
+  <si>
+    <t>ME water</t>
+  </si>
+  <si>
+    <t>ME propeller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME water </t>
+  </si>
+  <si>
+    <t xml:space="preserve">resulting equations </t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>x1x2</t>
+  </si>
+  <si>
+    <t>delay vs water =</t>
+  </si>
+  <si>
+    <t>delay vs propeller =</t>
+  </si>
+  <si>
+    <t>water vs propeller =</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>x1x3</t>
+  </si>
+  <si>
+    <t>x2x3</t>
+  </si>
+  <si>
+    <t>Resulting 2x2 relationship</t>
   </si>
 </sst>
 </file>
@@ -852,7 +978,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -860,11 +986,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -882,6 +1088,48 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -910,13 +1158,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>319089</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>138111</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>223838</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>-1</xdr:rowOff>
@@ -1020,13 +1268,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>138113</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
@@ -1168,15 +1416,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>61911</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>33336</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1273,16 +1521,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>14290</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>4765</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>200027</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1291,8 +1539,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6862765" y="6157914"/>
-          <a:ext cx="3052762" cy="1095374"/>
+          <a:off x="6672265" y="3252788"/>
+          <a:ext cx="3043235" cy="1771649"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1351,6 +1599,96 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t>-propeller	curved w/slit 1	flat w/o slit -1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>delay is x1 </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>water is x2 </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>propeller is x3</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>633416</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="633416" y="3776663"/>
+          <a:ext cx="2895597" cy="619125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Attempted to make</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> a 3x2 relationship, but cannot plot that on Matlab like rylander did</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -1836,10 +2174,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH45"/>
+  <dimension ref="A1:AK59"/>
   <sheetViews>
-    <sheetView topLeftCell="L7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AD9" sqref="AD9:AD16"/>
+    <sheetView tabSelected="1" topLeftCell="H32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1847,21 +2185,24 @@
     <col min="1" max="1" width="13.15625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.89453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.15625" customWidth="1"/>
-    <col min="4" max="4" width="4.578125" customWidth="1"/>
-    <col min="5" max="5" width="5" customWidth="1"/>
-    <col min="6" max="6" width="6.41796875" customWidth="1"/>
-    <col min="7" max="7" width="5.47265625" customWidth="1"/>
-    <col min="8" max="14" width="8.83984375" customWidth="1"/>
-    <col min="16" max="16" width="13.15625" bestFit="1" customWidth="1"/>
-    <col min="17" max="24" width="8.83984375" customWidth="1"/>
+    <col min="4" max="4" width="9.1015625" customWidth="1"/>
+    <col min="5" max="5" width="10.68359375" customWidth="1"/>
+    <col min="6" max="6" width="5" customWidth="1"/>
+    <col min="7" max="7" width="9.68359375" customWidth="1"/>
+    <col min="8" max="8" width="9.7890625" customWidth="1"/>
+    <col min="9" max="9" width="8.41796875" customWidth="1"/>
+    <col min="10" max="10" width="5.47265625" customWidth="1"/>
+    <col min="11" max="17" width="8.83984375" customWidth="1"/>
+    <col min="19" max="19" width="13.15625" customWidth="1"/>
+    <col min="20" max="27" width="8.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1872,7 +2213,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1883,7 +2224,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1894,7 +2235,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1905,46 +2246,46 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="H7" s="8" t="s">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="K7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
+      <c r="U7" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="V7" s="7"/>
       <c r="W7" s="7"/>
       <c r="X7" s="7"/>
       <c r="Y7" s="7"/>
-      <c r="Z7" s="4" t="s">
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AA7" s="4"/>
-      <c r="AB7" s="4"/>
-      <c r="AC7" s="5" t="s">
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AD7" s="5"/>
-      <c r="AE7" s="5"/>
-      <c r="AF7" s="6" t="s">
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="AG7" s="6"/>
-      <c r="AH7" s="6"/>
-    </row>
-    <row r="8" spans="1:34" ht="17.7" x14ac:dyDescent="0.75">
+      <c r="AJ7" s="6"/>
+      <c r="AK7" s="6"/>
+    </row>
+    <row r="8" spans="1:37" ht="17.7" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1961,73 +2302,73 @@
         <v>9</v>
       </c>
       <c r="F8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" t="s">
         <v>10</v>
       </c>
-      <c r="G8" t="s">
+      <c r="J8" t="s">
         <v>27</v>
       </c>
-      <c r="H8" t="s">
+      <c r="K8" t="s">
         <v>28</v>
       </c>
-      <c r="I8" t="s">
+      <c r="L8" t="s">
         <v>30</v>
       </c>
-      <c r="J8" t="s">
+      <c r="M8" t="s">
         <v>43</v>
       </c>
-      <c r="K8" t="s">
+      <c r="N8" t="s">
         <v>29</v>
       </c>
-      <c r="L8" t="s">
+      <c r="O8" t="s">
         <v>45</v>
       </c>
-      <c r="M8" t="s">
+      <c r="P8" t="s">
         <v>12</v>
       </c>
-      <c r="N8" t="s">
+      <c r="Q8" t="s">
         <v>33</v>
       </c>
-      <c r="O8" t="s">
+      <c r="R8" t="s">
         <v>26</v>
       </c>
-      <c r="P8" t="s">
+      <c r="S8" t="s">
         <v>44</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="T8" t="s">
         <v>41</v>
       </c>
-      <c r="R8" t="s">
+      <c r="U8" t="s">
         <v>14</v>
       </c>
-      <c r="S8" t="s">
+      <c r="V8" t="s">
         <v>31</v>
       </c>
-      <c r="T8" t="s">
+      <c r="W8" t="s">
         <v>43</v>
       </c>
-      <c r="U8" t="s">
+      <c r="X8" t="s">
         <v>11</v>
       </c>
-      <c r="V8" t="s">
+      <c r="Y8" t="s">
         <v>48</v>
       </c>
-      <c r="W8" t="s">
+      <c r="Z8" t="s">
         <v>12</v>
       </c>
-      <c r="X8" t="s">
+      <c r="AA8" t="s">
         <v>34</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="AB8" t="s">
         <v>13</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>19</v>
       </c>
       <c r="AC8" t="s">
         <v>18</v>
@@ -2047,8 +2388,17 @@
       <c r="AH8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+      <c r="AI8" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="9">
         <v>43211.081944444442</v>
       </c>
@@ -2065,108 +2415,120 @@
         <v>-1</v>
       </c>
       <c r="F9">
+        <f>C9*D9</f>
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f>C9*E9</f>
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <f>D9*E9</f>
+        <v>1</v>
+      </c>
+      <c r="I9">
         <f>C9*D9*E9</f>
         <v>-1</v>
       </c>
-      <c r="G9">
+      <c r="J9">
         <v>513</v>
       </c>
-      <c r="H9">
+      <c r="K9">
         <v>256</v>
       </c>
-      <c r="I9" t="s">
+      <c r="L9" t="s">
         <v>35</v>
       </c>
-      <c r="J9">
+      <c r="M9">
         <v>77</v>
       </c>
-      <c r="K9">
+      <c r="N9">
         <v>247</v>
       </c>
-      <c r="L9">
-        <f>(G9-H9)-(K9-J9)</f>
+      <c r="O9">
+        <f>(J9-K9)-(N9-M9)</f>
         <v>87</v>
       </c>
-      <c r="M9">
+      <c r="P9">
         <v>0.27</v>
       </c>
-      <c r="N9">
+      <c r="Q9">
         <v>66.39</v>
       </c>
-      <c r="O9">
+      <c r="R9">
         <f>(740730-121134)/1000</f>
         <v>619.596</v>
       </c>
-      <c r="P9" s="1">
+      <c r="S9" s="1">
         <v>43202.181250000001</v>
       </c>
-      <c r="Q9">
+      <c r="T9">
         <v>512</v>
       </c>
-      <c r="R9">
+      <c r="U9">
         <v>268</v>
       </c>
-      <c r="S9" t="s">
+      <c r="V9" t="s">
         <v>42</v>
       </c>
-      <c r="T9">
+      <c r="W9">
         <v>25</v>
       </c>
-      <c r="U9">
+      <c r="X9">
         <v>210</v>
       </c>
-      <c r="V9">
-        <f>(Q9-R9)-(U9-T9)</f>
+      <c r="Y9">
+        <f>(T9-U9)-(X9-W9)</f>
         <v>59</v>
       </c>
-      <c r="W9">
+      <c r="Z9">
         <v>0.26</v>
       </c>
-      <c r="X9">
+      <c r="AA9">
         <v>51.66</v>
       </c>
-      <c r="Y9">
+      <c r="AB9">
         <f>(589783-143635)/1000</f>
         <v>446.14800000000002</v>
       </c>
-      <c r="Z9">
-        <f>AVERAGE(O9,Y9)</f>
+      <c r="AC9">
+        <f>AVERAGE(R9,AB9)</f>
         <v>532.87200000000007</v>
       </c>
-      <c r="AA9">
-        <f>((O9-Z9)^2+(Y9-Z9)^2)/(2-1)</f>
+      <c r="AD9">
+        <f>((R9-AC9)^2+(AB9-AC9)^2)/(2-1)</f>
         <v>15042.104351999997</v>
-      </c>
-      <c r="AB9">
-        <f>SQRT(AA9)</f>
-        <v>122.64625698324429</v>
-      </c>
-      <c r="AC9">
-        <f>AVERAGE(L9,V9)</f>
-        <v>73</v>
-      </c>
-      <c r="AD9">
-        <f>((L9-AC9)^2+(V9-AC9)^2)/(2-1)</f>
-        <v>392</v>
       </c>
       <c r="AE9">
         <f>SQRT(AD9)</f>
-        <v>19.798989873223331</v>
+        <v>122.64625698324429</v>
       </c>
       <c r="AF9">
-        <f>AVERAGE(N9,X9)</f>
-        <v>59.024999999999999</v>
+        <f t="shared" ref="AF9:AF16" si="0">AVERAGE(O9,Y9)</f>
+        <v>73</v>
       </c>
       <c r="AG9">
-        <f>((N9-AF9)^2+(X9-AF9)^2)/(2-1)</f>
-        <v>108.48645000000006</v>
+        <f>((O9-AF9)^2+(Y9-AF9)^2)/(2-1)</f>
+        <v>392</v>
       </c>
       <c r="AH9">
         <f>SQRT(AG9)</f>
+        <v>19.798989873223331</v>
+      </c>
+      <c r="AI9">
+        <f>AVERAGE(Q9,AA9)</f>
+        <v>59.024999999999999</v>
+      </c>
+      <c r="AJ9">
+        <f>((Q9-AI9)^2+(AA9-AI9)^2)/(2-1)</f>
+        <v>108.48645000000006</v>
+      </c>
+      <c r="AK9">
+        <f>SQRT(AJ9)</f>
         <v>10.415682886877848</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>43211.094444444447</v>
       </c>
@@ -2183,109 +2545,121 @@
         <v>-1</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10:F16" si="0">C10*D10*E10</f>
+        <f t="shared" ref="F10:F16" si="1">C10*D10</f>
+        <v>-1</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ref="G10:G16" si="2">C10*E10</f>
+        <v>-1</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ref="H10:H16" si="3">D10*E10</f>
         <v>1</v>
       </c>
-      <c r="G10">
+      <c r="I10">
+        <f t="shared" ref="I10:I16" si="4">C10*D10*E10</f>
+        <v>1</v>
+      </c>
+      <c r="J10">
         <v>521</v>
       </c>
-      <c r="H10">
+      <c r="K10">
         <v>261</v>
       </c>
-      <c r="I10" t="s">
+      <c r="L10" t="s">
         <v>0</v>
       </c>
-      <c r="J10">
+      <c r="M10">
         <v>25</v>
       </c>
-      <c r="K10">
+      <c r="N10">
         <v>220</v>
       </c>
-      <c r="L10">
-        <f t="shared" ref="L10:L16" si="1">(G10-H10)-(K10-J10)</f>
+      <c r="O10">
+        <f t="shared" ref="O10:O16" si="5">(J10-K10)-(N10-M10)</f>
         <v>65</v>
       </c>
-      <c r="M10">
+      <c r="P10">
         <v>0.28000000000000003</v>
       </c>
-      <c r="N10">
+      <c r="Q10">
         <v>66.67</v>
       </c>
-      <c r="O10">
+      <c r="R10">
         <f>(595490-168671)/1000</f>
         <v>426.81900000000002</v>
       </c>
-      <c r="P10" s="1">
+      <c r="S10" s="1">
         <v>43211.166666666664</v>
       </c>
-      <c r="Q10">
+      <c r="T10">
         <v>516</v>
       </c>
-      <c r="R10">
+      <c r="U10">
         <v>271</v>
       </c>
-      <c r="S10" t="s">
+      <c r="V10" t="s">
         <v>42</v>
       </c>
-      <c r="T10">
+      <c r="W10">
         <v>25</v>
       </c>
-      <c r="U10">
+      <c r="X10">
         <v>213</v>
       </c>
-      <c r="V10">
-        <f t="shared" ref="V10:V16" si="2">(Q10-R10)-(U10-T10)</f>
+      <c r="Y10">
+        <f t="shared" ref="Y10:Y16" si="6">(T10-U10)-(X10-W10)</f>
         <v>57</v>
       </c>
-      <c r="W10">
+      <c r="Z10">
         <f>0.27</f>
         <v>0.27</v>
       </c>
-      <c r="X10">
+      <c r="AA10">
         <v>67.73</v>
       </c>
-      <c r="Y10">
+      <c r="AB10">
         <f>(1157316-619644)/1000</f>
         <v>537.67200000000003</v>
       </c>
-      <c r="Z10">
-        <f t="shared" ref="Z10:Z16" si="3">AVERAGE(O10,Y10)</f>
+      <c r="AC10">
+        <f t="shared" ref="AC10:AC16" si="7">AVERAGE(R10,AB10)</f>
         <v>482.24549999999999</v>
       </c>
-      <c r="AA10">
-        <f t="shared" ref="AA10:AA16" si="4">((O10-Z10)^2+(Y10-Z10)^2)/(2-1)</f>
+      <c r="AD10">
+        <f t="shared" ref="AD10:AD16" si="8">((R10-AC10)^2+(AB10-AC10)^2)/(2-1)</f>
         <v>6144.1938045000006</v>
       </c>
-      <c r="AB10">
-        <f t="shared" ref="AB10:AB17" si="5">SQRT(AA10)</f>
+      <c r="AE10">
+        <f t="shared" ref="AE10:AE16" si="9">SQRT(AD10)</f>
         <v>78.384908014872352</v>
       </c>
-      <c r="AC10">
-        <f>AVERAGE(L10,V10)</f>
+      <c r="AF10">
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="AD10">
-        <f t="shared" ref="AD10:AD16" si="6">((L10-AC10)^2+(V10-AC10)^2)/(2-1)</f>
+      <c r="AG10">
+        <f t="shared" ref="AG10:AG16" si="10">((O10-AF10)^2+(Y10-AF10)^2)/(2-1)</f>
         <v>32</v>
       </c>
-      <c r="AE10">
-        <f t="shared" ref="AE10:AE16" si="7">SQRT(AD10)</f>
+      <c r="AH10">
+        <f t="shared" ref="AH10:AH16" si="11">SQRT(AG10)</f>
         <v>5.6568542494923806</v>
       </c>
-      <c r="AF10">
-        <f t="shared" ref="AF10:AF16" si="8">AVERAGE(N10,X10)</f>
+      <c r="AI10">
+        <f t="shared" ref="AI10:AI16" si="12">AVERAGE(Q10,AA10)</f>
         <v>67.2</v>
       </c>
-      <c r="AG10">
-        <f t="shared" ref="AG10:AG16" si="9">((N10-AF10)^2+(X10-AF10)^2)/(2-1)</f>
+      <c r="AJ10">
+        <f t="shared" ref="AJ10:AJ16" si="13">((Q10-AI10)^2+(AA10-AI10)^2)/(2-1)</f>
         <v>0.56180000000000241</v>
       </c>
-      <c r="AH10">
-        <f t="shared" ref="AH10:AH16" si="10">SQRT(AG10)</f>
+      <c r="AK10">
+        <f t="shared" ref="AK10:AK16" si="14">SQRT(AJ10)</f>
         <v>0.74953318805774194</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>43210.19027777778</v>
       </c>
@@ -2302,105 +2676,117 @@
         <v>-1</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G11">
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J11">
         <v>513</v>
       </c>
-      <c r="H11">
+      <c r="K11">
         <v>243</v>
       </c>
-      <c r="I11" t="s">
+      <c r="L11" t="s">
         <v>0</v>
       </c>
-      <c r="J11">
+      <c r="M11">
         <v>25</v>
       </c>
-      <c r="K11">
+      <c r="N11">
         <v>222</v>
       </c>
-      <c r="L11">
-        <f t="shared" si="1"/>
+      <c r="O11">
+        <f t="shared" si="5"/>
         <v>73</v>
       </c>
-      <c r="M11">
+      <c r="P11">
         <v>0.28000000000000003</v>
       </c>
-      <c r="N11">
+      <c r="Q11">
         <v>59.375</v>
       </c>
-      <c r="O11">
+      <c r="R11">
         <f>(695760-154635)/1000</f>
         <v>541.125</v>
       </c>
-      <c r="Q11">
+      <c r="T11">
         <v>508</v>
       </c>
-      <c r="R11">
+      <c r="U11">
         <v>246</v>
       </c>
-      <c r="S11" t="s">
+      <c r="V11" t="s">
         <v>42</v>
       </c>
-      <c r="T11">
+      <c r="W11">
         <v>25</v>
       </c>
-      <c r="U11">
+      <c r="X11">
         <v>233</v>
       </c>
-      <c r="V11">
-        <f t="shared" si="2"/>
+      <c r="Y11">
+        <f t="shared" si="6"/>
         <v>54</v>
       </c>
-      <c r="W11">
+      <c r="Z11">
         <v>0.28000000000000003</v>
       </c>
-      <c r="X11">
+      <c r="AA11">
         <v>70.266999999999996</v>
       </c>
-      <c r="Y11">
+      <c r="AB11">
         <f>(431110-54132)/1000</f>
         <v>376.97800000000001</v>
       </c>
-      <c r="Z11">
-        <f t="shared" si="3"/>
+      <c r="AC11">
+        <f t="shared" si="7"/>
         <v>459.05150000000003</v>
       </c>
-      <c r="AA11">
-        <f t="shared" si="4"/>
+      <c r="AD11">
+        <f t="shared" si="8"/>
         <v>13472.118804499998</v>
       </c>
-      <c r="AB11">
-        <f t="shared" si="5"/>
+      <c r="AE11">
+        <f t="shared" si="9"/>
         <v>116.06945681142821</v>
       </c>
-      <c r="AC11">
-        <f>AVERAGE(L11,V11)</f>
+      <c r="AF11">
+        <f t="shared" si="0"/>
         <v>63.5</v>
       </c>
-      <c r="AD11">
-        <f t="shared" si="6"/>
+      <c r="AG11">
+        <f t="shared" si="10"/>
         <v>180.5</v>
       </c>
-      <c r="AE11">
-        <f t="shared" si="7"/>
+      <c r="AH11">
+        <f t="shared" si="11"/>
         <v>13.435028842544403</v>
       </c>
-      <c r="AF11">
-        <f t="shared" si="8"/>
+      <c r="AI11">
+        <f t="shared" si="12"/>
         <v>64.820999999999998</v>
       </c>
-      <c r="AG11">
-        <f t="shared" si="9"/>
+      <c r="AJ11">
+        <f t="shared" si="13"/>
         <v>59.317831999999953</v>
       </c>
-      <c r="AH11">
-        <f t="shared" si="10"/>
+      <c r="AK11">
+        <f t="shared" si="14"/>
         <v>7.7018070606838727</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>43211.058333333334</v>
       </c>
@@ -2417,108 +2803,120 @@
         <v>-1</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="G12">
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+      <c r="J12">
         <v>510</v>
       </c>
-      <c r="H12">
+      <c r="K12">
         <v>250</v>
       </c>
-      <c r="I12" t="s">
+      <c r="L12" t="s">
         <v>1</v>
       </c>
-      <c r="J12">
+      <c r="M12">
         <v>26</v>
       </c>
-      <c r="K12">
+      <c r="N12">
         <v>215</v>
       </c>
-      <c r="L12">
-        <f t="shared" si="1"/>
+      <c r="O12">
+        <f t="shared" si="5"/>
         <v>71</v>
       </c>
-      <c r="M12">
+      <c r="P12">
         <v>0.27</v>
       </c>
-      <c r="N12">
+      <c r="Q12">
         <v>63.875</v>
       </c>
-      <c r="O12">
+      <c r="R12">
         <f>(455924-46133)/1000</f>
         <v>409.791</v>
       </c>
-      <c r="P12" s="1">
+      <c r="S12" s="1">
         <v>43211.15625</v>
       </c>
-      <c r="Q12">
+      <c r="T12">
         <v>506</v>
       </c>
-      <c r="R12">
+      <c r="U12">
         <v>252</v>
       </c>
-      <c r="S12" t="s">
+      <c r="V12" t="s">
         <v>1</v>
       </c>
-      <c r="T12">
+      <c r="W12">
         <v>26</v>
       </c>
-      <c r="U12">
+      <c r="X12">
         <v>214</v>
       </c>
-      <c r="V12">
-        <f t="shared" si="2"/>
+      <c r="Y12">
+        <f t="shared" si="6"/>
         <v>66</v>
       </c>
-      <c r="W12">
+      <c r="Z12">
         <v>0.27</v>
       </c>
-      <c r="X12">
+      <c r="AA12">
         <v>64.015600000000006</v>
       </c>
-      <c r="Y12">
+      <c r="AB12">
         <f>(1157316-619644)/1000</f>
         <v>537.67200000000003</v>
       </c>
-      <c r="Z12">
-        <f t="shared" si="3"/>
+      <c r="AC12">
+        <f t="shared" si="7"/>
         <v>473.73149999999998</v>
       </c>
-      <c r="AA12">
-        <f t="shared" si="4"/>
+      <c r="AD12">
+        <f t="shared" si="8"/>
         <v>8176.7750805000032</v>
       </c>
-      <c r="AB12">
-        <f t="shared" si="5"/>
+      <c r="AE12">
+        <f t="shared" si="9"/>
         <v>90.425522284916909</v>
       </c>
-      <c r="AC12">
-        <f>AVERAGE(L12,V12)</f>
+      <c r="AF12">
+        <f t="shared" si="0"/>
         <v>68.5</v>
       </c>
-      <c r="AD12">
-        <f t="shared" si="6"/>
+      <c r="AG12">
+        <f t="shared" si="10"/>
         <v>12.5</v>
       </c>
-      <c r="AE12">
-        <f t="shared" si="7"/>
+      <c r="AH12">
+        <f t="shared" si="11"/>
         <v>3.5355339059327378</v>
       </c>
-      <c r="AF12">
-        <f t="shared" si="8"/>
+      <c r="AI12">
+        <f t="shared" si="12"/>
         <v>63.945300000000003</v>
       </c>
-      <c r="AG12">
-        <f t="shared" si="9"/>
+      <c r="AJ12">
+        <f t="shared" si="13"/>
         <v>9.8841800000008823E-3</v>
       </c>
-      <c r="AH12">
-        <f t="shared" si="10"/>
+      <c r="AK12">
+        <f t="shared" si="14"/>
         <v>9.9419213434833023E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>43210.169444444444</v>
       </c>
@@ -2535,108 +2933,120 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G13">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J13">
         <v>521</v>
       </c>
-      <c r="H13">
+      <c r="K13">
         <v>260</v>
       </c>
-      <c r="I13" t="s">
+      <c r="L13" t="s">
         <v>0</v>
       </c>
-      <c r="J13">
+      <c r="M13">
         <v>25</v>
       </c>
-      <c r="K13">
+      <c r="N13">
         <v>210</v>
       </c>
-      <c r="L13">
-        <f t="shared" si="1"/>
+      <c r="O13">
+        <f t="shared" si="5"/>
         <v>76</v>
       </c>
-      <c r="M13">
+      <c r="P13">
         <v>0.27</v>
       </c>
-      <c r="N13">
+      <c r="Q13">
         <v>63.5625</v>
       </c>
-      <c r="O13">
+      <c r="R13">
         <f>(668955-268054)/1000</f>
         <v>400.90100000000001</v>
       </c>
-      <c r="P13" s="1">
+      <c r="S13" s="1">
         <v>43211.208333333336</v>
       </c>
-      <c r="Q13">
+      <c r="T13">
         <v>498</v>
       </c>
-      <c r="R13">
+      <c r="U13">
         <v>273</v>
       </c>
-      <c r="S13" t="s">
+      <c r="V13" t="s">
         <v>1</v>
       </c>
-      <c r="T13">
+      <c r="W13">
         <v>26</v>
       </c>
-      <c r="U13">
+      <c r="X13">
         <v>182</v>
       </c>
-      <c r="V13">
-        <f t="shared" si="2"/>
+      <c r="Y13">
+        <f t="shared" si="6"/>
         <v>69</v>
       </c>
-      <c r="W13">
+      <c r="Z13">
         <v>0.27</v>
       </c>
-      <c r="X13">
+      <c r="AA13">
         <v>62.92</v>
       </c>
-      <c r="Y13">
+      <c r="AB13">
         <f>(468113-125634)/1000</f>
         <v>342.47899999999998</v>
       </c>
-      <c r="Z13">
-        <f t="shared" si="3"/>
+      <c r="AC13">
+        <f t="shared" si="7"/>
         <v>371.69</v>
       </c>
-      <c r="AA13">
-        <f t="shared" si="4"/>
+      <c r="AD13">
+        <f t="shared" si="8"/>
         <v>1706.5650420000015</v>
       </c>
-      <c r="AB13">
-        <f t="shared" si="5"/>
+      <c r="AE13">
+        <f t="shared" si="9"/>
         <v>41.310592370480499</v>
       </c>
-      <c r="AC13">
-        <f>AVERAGE(L13,V13)</f>
+      <c r="AF13">
+        <f t="shared" si="0"/>
         <v>72.5</v>
       </c>
-      <c r="AD13">
-        <f t="shared" si="6"/>
+      <c r="AG13">
+        <f t="shared" si="10"/>
         <v>24.5</v>
       </c>
-      <c r="AE13">
-        <f t="shared" si="7"/>
+      <c r="AH13">
+        <f t="shared" si="11"/>
         <v>4.9497474683058327</v>
       </c>
-      <c r="AF13">
-        <f t="shared" si="8"/>
+      <c r="AI13">
+        <f t="shared" si="12"/>
         <v>63.241250000000001</v>
       </c>
-      <c r="AG13">
-        <f t="shared" si="9"/>
+      <c r="AJ13">
+        <f t="shared" si="13"/>
         <v>0.20640312499999891</v>
       </c>
-      <c r="AH13">
-        <f t="shared" si="10"/>
+      <c r="AK13">
+        <f t="shared" si="14"/>
         <v>0.45431610691235558</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>43210.15347222222</v>
       </c>
@@ -2653,107 +3063,119 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="G14">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+      <c r="J14">
         <v>514</v>
       </c>
-      <c r="H14">
+      <c r="K14">
         <v>243</v>
       </c>
-      <c r="I14" t="s">
+      <c r="L14" t="s">
         <v>1</v>
       </c>
-      <c r="J14">
+      <c r="M14">
         <v>26</v>
       </c>
-      <c r="K14">
+      <c r="N14">
         <v>223</v>
       </c>
-      <c r="L14">
-        <f t="shared" si="1"/>
+      <c r="O14">
+        <f t="shared" si="5"/>
         <v>74</v>
       </c>
-      <c r="M14">
+      <c r="P14">
         <v>0.27</v>
       </c>
-      <c r="N14">
+      <c r="Q14">
         <v>63.1875</v>
       </c>
-      <c r="O14">
+      <c r="R14">
         <v>424.09500000000003</v>
       </c>
-      <c r="P14" s="1">
+      <c r="S14" s="1">
         <v>43211.229166666664</v>
       </c>
-      <c r="Q14">
+      <c r="T14">
         <v>502</v>
       </c>
-      <c r="R14">
+      <c r="U14">
         <v>251</v>
       </c>
-      <c r="S14" t="s">
+      <c r="V14" t="s">
         <v>1</v>
       </c>
-      <c r="T14">
+      <c r="W14">
         <v>26</v>
       </c>
-      <c r="U14">
+      <c r="X14">
         <v>214</v>
       </c>
-      <c r="V14">
-        <f t="shared" si="2"/>
+      <c r="Y14">
+        <f t="shared" si="6"/>
         <v>63</v>
       </c>
-      <c r="W14">
+      <c r="Z14">
         <v>0.27</v>
       </c>
-      <c r="X14">
+      <c r="AA14">
         <v>66.9375</v>
       </c>
-      <c r="Y14">
+      <c r="AB14">
         <f>(1931393-1562166)/1000</f>
         <v>369.22699999999998</v>
       </c>
-      <c r="Z14">
-        <f t="shared" si="3"/>
+      <c r="AC14">
+        <f t="shared" si="7"/>
         <v>396.661</v>
       </c>
-      <c r="AA14">
-        <f t="shared" si="4"/>
+      <c r="AD14">
+        <f t="shared" si="8"/>
         <v>1505.2487120000028</v>
       </c>
-      <c r="AB14">
-        <f t="shared" si="5"/>
+      <c r="AE14">
+        <f t="shared" si="9"/>
         <v>38.797534870143522</v>
       </c>
-      <c r="AC14">
-        <f>AVERAGE(L14,V14)</f>
+      <c r="AF14">
+        <f t="shared" si="0"/>
         <v>68.5</v>
       </c>
-      <c r="AD14">
-        <f t="shared" si="6"/>
+      <c r="AG14">
+        <f t="shared" si="10"/>
         <v>60.5</v>
       </c>
-      <c r="AE14">
-        <f t="shared" si="7"/>
+      <c r="AH14">
+        <f t="shared" si="11"/>
         <v>7.7781745930520225</v>
       </c>
-      <c r="AF14">
-        <f t="shared" si="8"/>
+      <c r="AI14">
+        <f t="shared" si="12"/>
         <v>65.0625</v>
       </c>
-      <c r="AG14">
-        <f t="shared" si="9"/>
+      <c r="AJ14">
+        <f t="shared" si="13"/>
         <v>7.03125</v>
       </c>
-      <c r="AH14">
-        <f t="shared" si="10"/>
+      <c r="AK14">
+        <f t="shared" si="14"/>
         <v>2.6516504294495533</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
         <v>43210.085416666669</v>
       </c>
@@ -2770,107 +3192,119 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="G15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+      <c r="J15">
         <v>520</v>
       </c>
-      <c r="H15">
+      <c r="K15">
         <v>285</v>
       </c>
-      <c r="I15" t="s">
+      <c r="L15" t="s">
         <v>0</v>
       </c>
-      <c r="J15">
+      <c r="M15">
         <v>25</v>
       </c>
-      <c r="K15">
+      <c r="N15">
         <v>168</v>
       </c>
-      <c r="L15">
-        <f t="shared" si="1"/>
+      <c r="O15">
+        <f t="shared" si="5"/>
         <v>92</v>
       </c>
-      <c r="M15">
+      <c r="P15">
         <v>0.26</v>
       </c>
-      <c r="N15">
+      <c r="Q15">
         <v>53.1875</v>
       </c>
-      <c r="O15">
+      <c r="R15">
         <v>523.80499999999995</v>
       </c>
-      <c r="P15" s="1">
+      <c r="S15" s="1">
         <v>43211.270833333336</v>
       </c>
-      <c r="Q15">
+      <c r="T15">
         <v>510</v>
       </c>
-      <c r="R15">
+      <c r="U15">
         <v>269</v>
       </c>
-      <c r="S15" t="s">
+      <c r="V15" t="s">
         <v>42</v>
       </c>
-      <c r="T15">
+      <c r="W15">
         <v>25</v>
       </c>
-      <c r="U15">
+      <c r="X15">
         <v>200</v>
       </c>
-      <c r="V15">
-        <f t="shared" si="2"/>
+      <c r="Y15">
+        <f t="shared" si="6"/>
         <v>66</v>
       </c>
-      <c r="W15">
+      <c r="Z15">
         <v>0.27</v>
       </c>
-      <c r="X15">
+      <c r="AA15">
         <v>71.625</v>
       </c>
-      <c r="Y15">
+      <c r="AB15">
         <f>(535961-126134)/1000</f>
         <v>409.827</v>
       </c>
-      <c r="Z15">
-        <f t="shared" si="3"/>
+      <c r="AC15">
+        <f t="shared" si="7"/>
         <v>466.81599999999997</v>
       </c>
-      <c r="AA15">
-        <f t="shared" si="4"/>
+      <c r="AD15">
+        <f t="shared" si="8"/>
         <v>6495.4922419999948</v>
       </c>
-      <c r="AB15">
-        <f t="shared" si="5"/>
+      <c r="AE15">
+        <f t="shared" si="9"/>
         <v>80.594616706080288</v>
       </c>
-      <c r="AC15">
-        <f>AVERAGE(L15,V15)</f>
+      <c r="AF15">
+        <f t="shared" si="0"/>
         <v>79</v>
       </c>
-      <c r="AD15">
-        <f t="shared" si="6"/>
+      <c r="AG15">
+        <f t="shared" si="10"/>
         <v>338</v>
       </c>
-      <c r="AE15">
-        <f t="shared" si="7"/>
+      <c r="AH15">
+        <f t="shared" si="11"/>
         <v>18.384776310850235</v>
       </c>
-      <c r="AF15">
-        <f t="shared" si="8"/>
+      <c r="AI15">
+        <f t="shared" si="12"/>
         <v>62.40625</v>
       </c>
-      <c r="AG15">
-        <f t="shared" si="9"/>
+      <c r="AJ15">
+        <f t="shared" si="13"/>
         <v>169.970703125</v>
       </c>
-      <c r="AH15">
-        <f t="shared" si="10"/>
+      <c r="AK15">
+        <f t="shared" si="14"/>
         <v>13.03728127812697</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3">
         <v>43210.151388888888</v>
       </c>
@@ -2887,143 +3321,158 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J16">
         <v>505</v>
       </c>
-      <c r="H16">
+      <c r="K16">
         <v>247</v>
       </c>
-      <c r="I16" t="s">
+      <c r="L16" t="s">
         <v>35</v>
       </c>
-      <c r="J16">
+      <c r="M16">
         <v>77</v>
       </c>
-      <c r="K16">
+      <c r="N16">
         <v>264</v>
       </c>
-      <c r="L16">
-        <f t="shared" si="1"/>
+      <c r="O16">
+        <f t="shared" si="5"/>
         <v>71</v>
       </c>
-      <c r="M16">
+      <c r="P16">
         <v>0.27</v>
       </c>
-      <c r="N16">
+      <c r="Q16">
         <v>64.75</v>
       </c>
-      <c r="O16">
+      <c r="R16">
         <f>(559365-137634)/1000</f>
         <v>421.73099999999999</v>
       </c>
-      <c r="P16" s="1">
+      <c r="S16" s="1">
         <v>43211.244444444441</v>
       </c>
-      <c r="Q16">
+      <c r="T16">
         <v>505</v>
       </c>
-      <c r="R16">
+      <c r="U16">
         <v>249</v>
       </c>
-      <c r="S16" t="s">
+      <c r="V16" t="s">
         <v>42</v>
       </c>
-      <c r="T16">
+      <c r="W16">
         <v>25</v>
       </c>
-      <c r="U16">
+      <c r="X16">
         <v>220</v>
       </c>
-      <c r="V16">
-        <f t="shared" si="2"/>
+      <c r="Y16">
+        <f t="shared" si="6"/>
         <v>61</v>
       </c>
-      <c r="W16">
+      <c r="Z16">
         <v>0.27</v>
       </c>
-      <c r="X16">
+      <c r="AA16">
         <v>62.09</v>
       </c>
-      <c r="Y16">
+      <c r="AB16">
         <f>(814747-434640)/1000</f>
         <v>380.10700000000003</v>
       </c>
-      <c r="Z16">
-        <f t="shared" si="3"/>
+      <c r="AC16">
+        <f t="shared" si="7"/>
         <v>400.91899999999998</v>
       </c>
-      <c r="AA16">
-        <f t="shared" si="4"/>
+      <c r="AD16">
+        <f t="shared" si="8"/>
         <v>866.27868799999862</v>
       </c>
-      <c r="AB16">
-        <f t="shared" si="5"/>
+      <c r="AE16">
+        <f t="shared" si="9"/>
         <v>29.43261266010883</v>
       </c>
-      <c r="AC16">
-        <f>AVERAGE(L16,V16)</f>
+      <c r="AF16">
+        <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="AD16">
-        <f t="shared" si="6"/>
+      <c r="AG16">
+        <f t="shared" si="10"/>
         <v>50</v>
       </c>
-      <c r="AE16">
-        <f t="shared" si="7"/>
+      <c r="AH16">
+        <f t="shared" si="11"/>
         <v>7.0710678118654755</v>
       </c>
-      <c r="AF16">
-        <f t="shared" si="8"/>
+      <c r="AI16">
+        <f t="shared" si="12"/>
         <v>63.42</v>
       </c>
-      <c r="AG16">
-        <f t="shared" si="9"/>
+      <c r="AJ16">
+        <f t="shared" si="13"/>
         <v>3.537799999999991</v>
       </c>
-      <c r="AH16">
-        <f t="shared" si="10"/>
+      <c r="AK16">
+        <f t="shared" si="14"/>
         <v>1.8809040379562141</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="14" t="s">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="Z17" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA17">
-        <f>SUM(AA9:AA16)/8</f>
-        <v>6676.0970906874991</v>
-      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
       <c r="AC17" t="s">
         <v>56</v>
       </c>
       <c r="AD17">
         <f>SUM(AD9:AD16)/8</f>
-        <v>136.25</v>
+        <v>6676.0970906874991</v>
       </c>
       <c r="AF17" t="s">
         <v>56</v>
       </c>
       <c r="AG17">
         <f>SUM(AG9:AG16)/8</f>
+        <v>136.25</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ17">
+        <f>SUM(AJ9:AJ16)/8</f>
         <v>43.640265303750006</v>
       </c>
     </row>
-    <row r="18" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="13" t="s">
+    <row r="18" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="24" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="13"/>
@@ -3037,38 +3486,38 @@
         <v>9</v>
       </c>
       <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
+      <c r="I18" s="25"/>
       <c r="Z18" s="2" t="s">
         <v>57</v>
       </c>
       <c r="AA18" s="2">
-        <f>SQRT(AA17)</f>
+        <f>SQRT(AD17)</f>
         <v>81.707387001956562</v>
       </c>
       <c r="AC18" s="2" t="s">
         <v>57</v>
       </c>
       <c r="AD18" s="2">
-        <f>SQRT(AD17)</f>
+        <f>SQRT(AG17)</f>
         <v>11.672617529928752</v>
       </c>
       <c r="AF18" s="2" t="s">
         <v>57</v>
       </c>
       <c r="AG18" s="2">
-        <f>SQRT(AG17)</f>
+        <f>SQRT(AJ17)</f>
         <v>6.6060779062731321</v>
       </c>
     </row>
-    <row r="19" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="11">
-        <f>AVERAGE(O9:O16,Y9:Y16)</f>
+        <f>AVERAGE(R9:R16,AB9:AB16)</f>
         <v>447.99831250000005</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -3078,7 +3527,7 @@
         <v>22</v>
       </c>
       <c r="F19" s="2">
-        <f>AVERAGE(O9:O16,Y9:Y16)</f>
+        <f>AVERAGE(R9:R16,AB9:AB16)</f>
         <v>447.99831250000005</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -3087,8 +3536,8 @@
       <c r="H19" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="11">
-        <f>AVERAGE(O9:O16,Y9:Y16)</f>
+      <c r="I19" s="26">
+        <f>AVERAGE(R9:R16,AB9:AB16)</f>
         <v>447.99831250000005</v>
       </c>
       <c r="Z19" s="2" t="s">
@@ -3113,15 +3562,15 @@
         <v>1.651519476568283</v>
       </c>
     </row>
-    <row r="20" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="11">
-        <f>AVERAGE(O10,O12,O15:O16,Y10,Y12,Y15:Y16)-AVERAGE(O9,O11,O13:O14,Y9,Y11,Y13:Y14)</f>
+        <f>AVERAGE(R10,R12,R15:R16,AB10,AB12,AB15:AB16)-AVERAGE(R9,R11,R13:R14,AB9,AB11,AB13:AB14)</f>
         <v>15.859375</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -3131,7 +3580,7 @@
         <v>38</v>
       </c>
       <c r="F20" s="2">
-        <f>AVERAGE(O11,O12,O14,O16,Y11,Y12,Y14,Y16)-AVERAGE(O9,O10,O13,O15,Y9,Y10,Y13,Y15)</f>
+        <f>AVERAGE(R11,R12,R14,R16,AB11,AB12,AB14,AB16)-AVERAGE(R9,R10,R13,R15,AB9,AB10,AB13,AB15)</f>
         <v>-30.81512500000008</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -3140,8 +3589,8 @@
       <c r="H20" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="I20" s="11">
-        <f>AVERAGE(O13:O16,Y13:Y16)-AVERAGE(O9:O12,Y9:Y12)</f>
+      <c r="I20" s="26">
+        <f>AVERAGE(R13:R16,AB13:AB16)-AVERAGE(R9:R12,AB9:AB12)</f>
         <v>-77.953625000000045</v>
       </c>
       <c r="Z20" s="10" t="s">
@@ -3166,123 +3615,120 @@
         <v>3.303038953136566</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="12">
-        <f>AVERAGE(O10,O11,O13,O16,Y10,Y11,Y13,Y16)-AVERAGE(O9,O12,O14:O15,Y9,Y12,Y14:Y15)</f>
+      <c r="C21" s="11">
+        <f>AVERAGE(R10,R11,R13,R16,AB10,AB11,AB13,AB16)-AVERAGE(R9,R12,R14:R15,AB9,AB12,AB14:AB15)</f>
         <v>-39.04362500000002</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F21">
-        <f>AVERAGE(O10,O11,O13,O16,Y10,Y11,Y13,Y16)-AVERAGE(O9,O12,O14,O15,Y9,Y12,Y14,Y15)</f>
+      <c r="F21" s="2">
+        <f>AVERAGE(R10,R11,R13,R16,AB10,AB11,AB13,AB16)-AVERAGE(R9,R12,R14,R15,AB9,AB12,AB14,AB15)</f>
         <v>-39.04362500000002</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I21" s="12">
-        <f>AVERAGE(O10,O11,O13,O16,Y10,Y11,Y13,Y16)-AVERAGE(O9,O12,O14,O15,Y9,Y12,Y14,Y15)</f>
+      <c r="I21" s="26">
+        <f>AVERAGE(R10,R11,R13,R16,AB10,AB11,AB13,AB16)-AVERAGE(R9,R12,R14,R15,AB9,AB12,AB14,AB15)</f>
         <v>-39.04362500000002</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="11">
         <f>C20/2</f>
         <v>7.9296875</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <f>F20/2</f>
         <v>-15.40756250000004</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I22" s="12">
+      <c r="I22" s="26">
         <f>I20/2</f>
         <v>-38.976812500000023</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="11">
         <f>C21/2</f>
         <v>-19.52181250000001</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2">
         <f>F21/2</f>
         <v>-19.52181250000001</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="12">
+      <c r="I23" s="26">
         <f>I21/2</f>
         <v>-19.52181250000001</v>
       </c>
-      <c r="Z23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="14" t="s">
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="Z24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="13" t="s">
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="24" t="s">
         <v>8</v>
       </c>
       <c r="B25" s="13"/>
@@ -3296,20 +3742,17 @@
         <v>9</v>
       </c>
       <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="Z25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="2" t="s">
+      <c r="I25" s="25"/>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C26" s="11">
-        <f>AVERAGE(N9:N16,X9:X16)</f>
+        <f>AVERAGE(Q9:Q16,AA9:AA16)</f>
         <v>63.640162500000002</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -3319,7 +3762,7 @@
         <v>22</v>
       </c>
       <c r="F26" s="11">
-        <f>AVERAGE(N9:N16,X9:X16)</f>
+        <f>AVERAGE(Q9:Q16,AA9:AA16)</f>
         <v>63.640162500000002</v>
       </c>
       <c r="G26" s="2" t="s">
@@ -3328,23 +3771,20 @@
       <c r="H26" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="11">
-        <f>AVERAGE(N9:N16,X9:X16)</f>
+      <c r="I26" s="26">
+        <f>AVERAGE(Q9:Q16,AA9:AA16)</f>
         <v>63.640162500000002</v>
       </c>
-      <c r="Z26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="2" t="s">
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="11">
-        <f>AVERAGE(N10,N12,N15:N16,X10,X12,X15:X16)-AVERAGE(N9,N11,N13:N14,X9,X11,X13:X14)</f>
+        <f>AVERAGE(Q10,Q12,Q15:Q16,AA10,AA12,AA15:AA16)-AVERAGE(Q9,Q11,Q13:Q14,AA9,AA11,AA13:AA14)</f>
         <v>1.2054500000000132</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -3354,7 +3794,7 @@
         <v>38</v>
       </c>
       <c r="F27" s="11">
-        <f>AVERAGE(N11:N12,N14,N16,X11:X12,X14,X16)-AVERAGE(N9:N10,N13,N15,X9:X10,X13,X15)</f>
+        <f>AVERAGE(Q11:Q12,Q14,Q16,AA11:AA12,AA14,AA16)-AVERAGE(Q9:Q10,Q13,Q15,AA9:AA10,AA13,AA15)</f>
         <v>1.3440749999999966</v>
       </c>
       <c r="G27" s="2" t="s">
@@ -3363,131 +3803,125 @@
       <c r="H27" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="I27" s="11">
-        <f>AVERAGE(N13:N16,X13:X16)-AVERAGE(N9:N12,X9:X12)</f>
+      <c r="I27" s="26">
+        <f>AVERAGE(Q13:Q16,AA13:AA16)-AVERAGE(Q9:Q12,AA9:AA12)</f>
         <v>-0.21532500000000709</v>
       </c>
-      <c r="Z27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="12">
-        <f>AVERAGE(N10:N11,N13,N16,X10:X11,X13,X16)-AVERAGE(N9,N12,N14:N15,X9,X12,X14:X15)</f>
+      <c r="C28" s="11">
+        <f>AVERAGE(Q10:Q11,Q13,Q16,AA10:AA11,AA13,AA16)-AVERAGE(Q9,Q12,Q14:Q15,AA9,AA12,AA14:AA15)</f>
         <v>2.0608000000000075</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="12">
-        <f>AVERAGE(N10:N11,N13,N16,X10:X11,X13,X16)-AVERAGE(N9,N12,N14:N15,X9,X12,X14:X15)</f>
+      <c r="F28" s="11">
+        <f>AVERAGE(Q10:Q11,Q13,Q16,AA10:AA11,AA13,AA16)-AVERAGE(Q9,Q12,Q14:Q15,AA9,AA12,AA14:AA15)</f>
         <v>2.0608000000000075</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I28" s="12">
-        <f>AVERAGE(N10,N11,N13,N16,X10:X11,X13,X16)-AVERAGE(N9,N12,N14:N15,X9,X12,X14:X15)</f>
+      <c r="I28" s="26">
+        <f>AVERAGE(Q10,Q11,Q13,Q16,AA10:AA11,AA13,AA16)-AVERAGE(Q9,Q12,Q14:Q15,AA9,AA12,AA14:AA15)</f>
         <v>2.0608000000000075</v>
       </c>
-      <c r="Z28" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C29" s="11">
         <f>C27/2</f>
         <v>0.60272500000000662</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F29" s="12">
+      <c r="F29" s="11">
         <f>F27/2</f>
         <v>0.67203749999999829</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I29" s="12">
+      <c r="I29" s="26">
         <f>I27/2</f>
         <v>-0.10766250000000355</v>
       </c>
-      <c r="Z29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="11">
         <f>C28/2</f>
         <v>1.0304000000000038</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="12">
+      <c r="F30" s="11">
         <f>F28/2</f>
         <v>1.0304000000000038</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I30" s="12">
+      <c r="I30" s="26">
         <f>I28/2</f>
         <v>1.0304000000000038</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="14" t="s">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-    </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="13" t="s">
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="24" t="s">
         <v>8</v>
       </c>
       <c r="B32" s="13"/>
@@ -3501,17 +3935,17 @@
         <v>9</v>
       </c>
       <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="2" t="s">
+      <c r="I32" s="25"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C33" s="11">
-        <f>AVERAGE(L9:L16,V9:V16)</f>
+        <f>AVERAGE(O9:O16,Y9:Y16)</f>
         <v>69</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -3521,7 +3955,7 @@
         <v>22</v>
       </c>
       <c r="F33" s="11">
-        <f>AVERAGE(L9:L16,V9:V16)</f>
+        <f>AVERAGE(O9:O16,Y9:Y16)</f>
         <v>69</v>
       </c>
       <c r="G33" s="2" t="s">
@@ -3530,20 +3964,20 @@
       <c r="H33" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I33" s="11">
-        <f>AVERAGE(L9:L16,V9:V16)</f>
+      <c r="I33" s="26">
+        <f>AVERAGE(O9:O16,Y9:Y16)</f>
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C34" s="11">
-        <f>AVERAGE(L10,L12,L15:L16,V10,V12,V15:V16)-AVERAGE(L9,L11,L13:L14,V9,V11,V13:V14)</f>
+        <f>AVERAGE(O10,O12,O15:O16,Y10,Y12,Y15:Y16)-AVERAGE(O9,O11,O13:O14,Y9,Y11,Y13:Y14)</f>
         <v>-0.75</v>
       </c>
       <c r="D34" s="2" t="s">
@@ -3553,7 +3987,7 @@
         <v>38</v>
       </c>
       <c r="F34" s="11">
-        <f>AVERAGE(L11:L12,L14,L16,V11:V12,V14,V16)-AVERAGE(L9:L10,L13,L15,V9:V10,V13,V15)</f>
+        <f>AVERAGE(O11:O12,O14,O16,Y11:Y12,Y14,Y16)-AVERAGE(O9:O10,O13,O15,Y9:Y10,Y13,Y15)</f>
         <v>-4.75</v>
       </c>
       <c r="G34" s="2" t="s">
@@ -3562,156 +3996,936 @@
       <c r="H34" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="I34" s="11">
-        <f>AVERAGE(L13:L16,V13:V16)-AVERAGE(L9:L12,V9:V12)</f>
+      <c r="I34" s="26">
+        <f>AVERAGE(O13:O16,Y13:Y16)-AVERAGE(O9:O12,Y9:Y12)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C35" s="11">
-        <f>AVERAGE(L10,L11,L13,L16,V10,V11,V13,V16)-AVERAGE(L9,L12,L14:L15,V9,V12,V14:V15)</f>
+        <f>AVERAGE(O10,O11,O13,O16,Y10,Y11,Y13,Y16)-AVERAGE(O9,O12,O14:O15,Y9,Y12,Y14:Y15)</f>
         <v>-6.5</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F35" s="12">
-        <f>AVERAGE(V10,V11,V13,V16,L10,L11,L13,L16)-AVERAGE(L9,L12,L14:L15,V9,V12,V14:V15)</f>
+      <c r="F35" s="11">
+        <f>AVERAGE(Y10,Y11,Y13,Y16,O10,O11,O13,O16)-AVERAGE(O9,O12,O14:O15,Y9,Y12,Y14:Y15)</f>
         <v>-6.5</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I35" s="12">
-        <f>AVERAGE(L10:L11,L13,L16,V10:V11,V13,V16)-AVERAGE(L9,L12,L14:L15,V9,V12,V14:V15)</f>
+      <c r="I35" s="26">
+        <f>AVERAGE(O10:O11,O13,O16,Y10:Y11,Y13,Y16)-AVERAGE(O9,O12,O14:O15,Y9,Y12,Y14:Y15)</f>
         <v>-6.5</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="s">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="12">
+      <c r="C36" s="11">
         <f>C34/2</f>
         <v>-0.375</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F36" s="12">
+      <c r="F36" s="11">
         <f>F34/2</f>
         <v>-2.375</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I36" s="12">
+      <c r="I36" s="26">
         <f>I34/2</f>
         <v>2.5</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="12">
+      <c r="C37" s="30">
         <f>C35/2</f>
         <v>-3.25</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="F37" s="12">
+      <c r="F37" s="30">
         <f>F35/2</f>
         <v>-3.25</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="I37" s="12">
+      <c r="I37" s="31">
         <f>I35/2</f>
         <v>-3.25</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" t="s">
-        <v>55</v>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="34"/>
+      <c r="H40" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="33"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="33"/>
+      <c r="O40" s="33"/>
+      <c r="P40" s="33"/>
+      <c r="Q40" s="33"/>
+      <c r="R40" s="34"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F41" s="16"/>
+      <c r="H41" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="16"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" s="2">
+        <f>AVERAGE(R9:R16,AB9:AB16)</f>
+        <v>447.99831250000005</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="2">
+        <f>AVERAGE(R9:R16,AB9:AB16)</f>
+        <v>447.99831250000005</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F42" s="16">
+        <f>AVERAGE(R9:R16,AB9:AB16)</f>
+        <v>447.99831250000005</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="I42" s="2">
+        <f>B42</f>
+        <v>447.99831250000005</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K42" s="2">
+        <f>B43</f>
+        <v>15.859375</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N42" s="2">
+        <f>B44</f>
+        <v>-30.81512500000008</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q42" s="2">
+        <f>B45</f>
+        <v>-11.173312500000009</v>
+      </c>
+      <c r="R42" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="2">
+        <f>AVERAGE(R10,R12,R15:R16,AB10,AB12,AB15:AB16)-AVERAGE(R9,R11,R13:R14,AB9,AB11,AB13:AB14)</f>
+        <v>15.859375</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" s="2">
+        <f>AVERAGE(R10,R12,R15:R16,AB10,AB12,AB15:AB16)-AVERAGE(R9,R11,R13:R14,AB9,AB11,AB13:AB14)</f>
+        <v>15.859375</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F43" s="16">
+        <f>AVERAGE(R11:R12,R14,R16,AB11:AB12,AB14,AB16)-AVERAGE(R9:R10,R13,R15,AB9:AB10,AB13,AB15)</f>
+        <v>-30.81512500000008</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I43" s="2">
+        <f>D42</f>
+        <v>447.99831250000005</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K43" s="2">
+        <f>D43</f>
+        <v>15.859375</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N43" s="2">
+        <f>D44</f>
+        <v>-77.953625000000045</v>
+      </c>
+      <c r="O43" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="P43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q43" s="2">
+        <f>D45</f>
+        <v>72.497687499999984</v>
+      </c>
+      <c r="R43" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="2">
+        <f>AVERAGE(R11:R12,R14,R16,AB11:AB12,AB14,AB16)-AVERAGE(R9:R10,R13,R15,AB9:AB10,AB13,AB15)</f>
+        <v>-30.81512500000008</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D44" s="2">
+        <f>AVERAGE(R13:R16,AB13:AB16)-AVERAGE(R9:R12,AB9:AB12)</f>
+        <v>-77.953625000000045</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F44" s="16">
+        <f>AVERAGE(R13:R16,AB13:AB16)-AVERAGE(R9:R12,AB9:AB12)</f>
+        <v>-77.953625000000045</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="I44" s="2">
+        <f>F42</f>
+        <v>447.99831250000005</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K44" s="2">
+        <f>F43</f>
+        <v>-30.81512500000008</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N44" s="2">
+        <f>F44</f>
+        <v>-77.953625000000045</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q44" s="2">
+        <f>F45</f>
+        <v>7.253437500000075</v>
+      </c>
+      <c r="R44" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="2">
+        <f>AVERAGE(R9,R12:R13,R16,AC9,AC12:AC13,AC16)-AVERAGE(R10:R11,R14:R15,AC10:AC11,AC14:AC15)</f>
+        <v>-11.173312500000009</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45" s="2">
+        <f>AVERAGE(R9,R11,R15:R16,AC9,AC11,AC15:AC16)-AVERAGE(R10,R12:R14,AC10,AC12:AC14)</f>
+        <v>72.497687499999984</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F45" s="16">
+        <f>AVERAGE(R9:R10,R14,R16,AC9:AC10,AC14,AC16)-AVERAGE(R11:R13,R15,AC11:AC13,AC15)</f>
+        <v>7.253437500000075</v>
+      </c>
+      <c r="H45" s="15"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="16"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="15"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="16"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="16"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="25"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="16"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F48" s="16"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="16"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="2">
+        <f>AVERAGE(Q9:Q16,AA9:AA16)</f>
+        <v>63.640162500000002</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" s="2">
+        <f>AVERAGE(Q9:Q16,AA9:AA16)</f>
+        <v>63.640162500000002</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F49" s="16">
+        <f>AVERAGE(Q9:Q16,AA9:AA16)</f>
+        <v>63.640162500000002</v>
+      </c>
+      <c r="H49" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="I49" s="2">
+        <f>B49</f>
+        <v>63.640162500000002</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K49" s="2">
+        <f>B50</f>
+        <v>1.2054500000000132</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N49" s="2">
+        <f>B51</f>
+        <v>1.3440749999999966</v>
+      </c>
+      <c r="O49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q49" s="2">
+        <f>B52</f>
+        <v>-2.4645500000000027</v>
+      </c>
+      <c r="R49" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" s="2">
+        <f>AVERAGE(Q10,Q12,Q15:Q16,AA10,AA12,AA15:AA16)-AVERAGE(Q9,Q11,Q13:Q14,AA9,AA11,AA13:AA14)</f>
+        <v>1.2054500000000132</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" s="2">
+        <f>AVERAGE(Q10,Q12,Q15:Q16,AA10,AA12,AA15:AA16)-AVERAGE(Q9,Q11,Q13:Q14,AA9,AA11,AA13:AA14)</f>
+        <v>1.2054500000000132</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F50" s="16">
+        <f>AVERAGE(Q11:Q12,Q14,Q16,AA11:AA12,AA14,AA16)-AVERAGE(Q9:Q10,Q13,Q15,AA9:AA10,AA13,AA15)</f>
+        <v>1.3440749999999966</v>
+      </c>
+      <c r="H50" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I50" s="2">
+        <f>D49</f>
+        <v>63.640162500000002</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K50" s="2">
+        <f>D50</f>
+        <v>1.2054500000000132</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N50" s="2">
+        <f>D51</f>
+        <v>-0.21532500000000709</v>
+      </c>
+      <c r="O50" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="P50" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q50" s="2">
+        <f>D52</f>
+        <v>-2.4442000000000235</v>
+      </c>
+      <c r="R50" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51" s="2">
+        <f>AVERAGE(Q11:Q12,Q14,Q16,AA11:AA12,AA14,AA16)-AVERAGE(Q9:Q10,Q13,Q15,AA9:AA10,AA13,AA15)</f>
+        <v>1.3440749999999966</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D51" s="2">
+        <f>AVERAGE(Q13:Q16,AA13:AA16)-AVERAGE(Q9:Q12,AA9:AA12)</f>
+        <v>-0.21532500000000709</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F51" s="16">
+        <f>AVERAGE(Q13:Q16,AA13:AA16)-AVERAGE(Q9:Q12,AA9:AA12)</f>
+        <v>-0.21532500000000709</v>
+      </c>
+      <c r="H51" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="I51" s="2">
+        <f>F49</f>
+        <v>63.640162500000002</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K51" s="2">
+        <f>F50</f>
+        <v>1.3440749999999966</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N51" s="2">
+        <f>F51</f>
+        <v>-0.21532500000000709</v>
+      </c>
+      <c r="O51" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="P51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q51" s="2">
+        <f>F52</f>
+        <v>7.3425000000007401E-2</v>
+      </c>
+      <c r="R51" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="2">
+        <f>AVERAGE(Q9,Q12:Q13,Q16,AA9,AA12:AA13,AA16)-AVERAGE(Q10:Q11,Q14:Q15,AA10:AA11,AA14:AA15)</f>
+        <v>-2.4645500000000027</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D52" s="2">
+        <f>AVERAGE(Q9,Q11,Q15:Q16,AA9,AA11,AA15:AA16)-AVERAGE(Q10,Q12:Q14,AA10,AA12:AA14)</f>
+        <v>-2.4442000000000235</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F52" s="16">
+        <f>AVERAGE(Q9:Q10,Q14,Q16,AA9:AA10,AA14,AA16)-AVERAGE(Q11:Q13,Q15,AA11:AA13,AA15)</f>
+        <v>7.3425000000007401E-2</v>
+      </c>
+      <c r="H52" s="15"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="16"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="15"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="16"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="16"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="25"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" s="2"/>
+      <c r="P54" s="2"/>
+      <c r="Q54" s="2"/>
+      <c r="R54" s="16"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F55" s="16"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="2"/>
+      <c r="R55" s="16"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56" s="2">
+        <f>AVERAGE(O9:O16,Y9:Y16)</f>
+        <v>69</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D56" s="2">
+        <f>AVERAGE(O9:O16,Y9:Y16)</f>
+        <v>69</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F56" s="16">
+        <f>AVERAGE(O9:O16,Y9:Y16)</f>
+        <v>69</v>
+      </c>
+      <c r="H56" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="I56" s="2">
+        <f>B56</f>
+        <v>69</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K56" s="2">
+        <f>B57</f>
+        <v>-0.75</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N56" s="2">
+        <f>B58</f>
+        <v>-4.75</v>
+      </c>
+      <c r="O56" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P56" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q56" s="2">
+        <f>B59</f>
+        <v>2</v>
+      </c>
+      <c r="R56" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B57" s="2">
+        <f>AVERAGE(O10,O12,O15:O16,Y10,Y12,Y15:Y16)-AVERAGE(O9,O11,O13:O14,Y9,Y11,Y13:Y14)</f>
+        <v>-0.75</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D57" s="2">
+        <f>AVERAGE(O10,O12,O15:O16,Y10,Y12,Y15:Y16)-AVERAGE(O9,O11,O13:O14,Y9,Y11,Y13:Y14)</f>
+        <v>-0.75</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F57" s="16">
+        <f>AVERAGE(O11:O12,O14,O16,Y11:Y12,Y14,Y16)-AVERAGE(O9:O10,O13,O15,Y9:Y10,Y13,Y15)</f>
+        <v>-4.75</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I57" s="2">
+        <f>D56</f>
+        <v>69</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K57" s="2">
+        <f>D57</f>
+        <v>-0.75</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N57" s="2">
+        <f>D58</f>
+        <v>5</v>
+      </c>
+      <c r="O57" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="P57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q57" s="2">
+        <f>D59</f>
+        <v>2.75</v>
+      </c>
+      <c r="R57" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58" s="2">
+        <f>AVERAGE(O11:O12,O14,O16,Y11:Y12,Y14,Y16)-AVERAGE(O9:O10,O13,O15,Y9:Y10,Y13,Y15)</f>
+        <v>-4.75</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D58" s="2">
+        <f>AVERAGE(O13:O16,Y13:Y16)-AVERAGE(O9:O12,Y9:Y12)</f>
+        <v>5</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F58" s="16">
+        <f>AVERAGE(O13:O16,Y13:Y16)-AVERAGE(O9:O12,Y9:Y12)</f>
+        <v>5</v>
+      </c>
+      <c r="H58" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I58" s="18">
+        <f>F56</f>
+        <v>69</v>
+      </c>
+      <c r="J58" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="K58" s="18">
+        <f>F57</f>
+        <v>-4.75</v>
+      </c>
+      <c r="L58" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="M58" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="N58" s="18">
+        <f>F58</f>
+        <v>5</v>
+      </c>
+      <c r="O58" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="P58" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q58" s="18">
+        <f>F59</f>
+        <v>-3.75</v>
+      </c>
+      <c r="R58" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="18">
+        <f>AVERAGE(O9,O12:O13,O16,Y9,Y12:Y13,Y16)-AVERAGE(O10:O11,O14:O15,Y10:Y11,Y14:Y15)</f>
+        <v>2</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D59" s="18">
+        <f>AVERAGE(O9,O11,O15:O16,Y9,Y11,Y15:Y16)-AVERAGE(O10,O12:O14,Y10,Y12:Y14)</f>
+        <v>2.75</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F59" s="19">
+        <f>AVERAGE(O9:O10,O14,O16,Y9:Y10,Y14,Y16)-AVERAGE(O11:O13,O15,Y11:Y13,Y15)</f>
+        <v>-3.75</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="16">
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="H40:R40"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="A31:I31"/>
     <mergeCell ref="A18:C18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="G25:I25"/>
     <mergeCell ref="D18:F18"/>
-    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="A24:I24"/>
     <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="A24:I24"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="G32:I32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -3724,7 +4938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -4026,7 +5240,7 @@
         <v>33.836473693338654</v>
       </c>
       <c r="AC9">
-        <f>AVERAGE(L9,V9)</f>
+        <f t="shared" ref="AC9:AC16" si="0">AVERAGE(L9,V9)</f>
         <v>60</v>
       </c>
       <c r="AD9">
@@ -4067,7 +5281,7 @@
         <v>-1</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10:F16" si="0">C10*D10*E10</f>
+        <f t="shared" ref="F10:F16" si="1">C10*D10*E10</f>
         <v>1</v>
       </c>
       <c r="G10">
@@ -4116,7 +5330,7 @@
         <v>213</v>
       </c>
       <c r="V10">
-        <f t="shared" ref="V10:V16" si="1">(Q10-R10)-(U10-T10)</f>
+        <f t="shared" ref="V10:V16" si="2">(Q10-R10)-(U10-T10)</f>
         <v>57</v>
       </c>
       <c r="W10">
@@ -4131,39 +5345,39 @@
         <v>537.67200000000003</v>
       </c>
       <c r="Z10">
-        <f t="shared" ref="Z10:Z16" si="2">AVERAGE(O10,Y10)</f>
+        <f t="shared" ref="Z10:Z16" si="3">AVERAGE(O10,Y10)</f>
         <v>513.83600000000001</v>
       </c>
       <c r="AA10">
-        <f t="shared" ref="AA10:AA16" si="3">((O10-Z10)^2+(Y10-Z10)^2)/(2-1)</f>
+        <f t="shared" ref="AA10:AA16" si="4">((O10-Z10)^2+(Y10-Z10)^2)/(2-1)</f>
         <v>1136.3097920000012</v>
       </c>
       <c r="AB10">
-        <f t="shared" ref="AB10:AB17" si="4">SQRT(AA10)</f>
+        <f t="shared" ref="AB10:AB16" si="5">SQRT(AA10)</f>
         <v>33.709194472725109</v>
       </c>
       <c r="AC10">
-        <f>AVERAGE(L10,V10)</f>
+        <f t="shared" si="0"/>
         <v>58.5</v>
       </c>
       <c r="AD10">
-        <f t="shared" ref="AD10:AD16" si="5">((L10-AC10)^2+(V10-AC10)^2)/(2-1)</f>
+        <f t="shared" ref="AD10:AD16" si="6">((L10-AC10)^2+(V10-AC10)^2)/(2-1)</f>
         <v>4.5</v>
       </c>
       <c r="AE10">
-        <f t="shared" ref="AE10:AE16" si="6">SQRT(AD10)</f>
+        <f t="shared" ref="AE10:AE16" si="7">SQRT(AD10)</f>
         <v>2.1213203435596424</v>
       </c>
       <c r="AF10">
-        <f t="shared" ref="AF10:AF16" si="7">AVERAGE(N10,X10)</f>
+        <f t="shared" ref="AF10:AF16" si="8">AVERAGE(N10,X10)</f>
         <v>66.865000000000009</v>
       </c>
       <c r="AG10">
-        <f t="shared" ref="AG10:AG16" si="8">((N10-AF10)^2+(X10-AF10)^2)/(2-1)</f>
+        <f t="shared" ref="AG10:AG16" si="9">((N10-AF10)^2+(X10-AF10)^2)/(2-1)</f>
         <v>1.4964500000000069</v>
       </c>
       <c r="AH10">
-        <f t="shared" ref="AH10:AH16" si="9">SQRT(AG10)</f>
+        <f t="shared" ref="AH10:AH16" si="10">SQRT(AG10)</f>
         <v>1.22329473145273</v>
       </c>
     </row>
@@ -4184,7 +5398,7 @@
         <v>-1</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G11">
@@ -4230,7 +5444,7 @@
         <v>233</v>
       </c>
       <c r="V11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="W11">
@@ -4244,39 +5458,39 @@
         <v>376.97800000000001</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>398.48900000000003</v>
       </c>
       <c r="AA11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>925.44624199999953</v>
       </c>
       <c r="AB11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30.421147940207639</v>
       </c>
       <c r="AC11">
-        <f>AVERAGE(L11,V11)</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="AD11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="AE11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="AF11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>69.633499999999998</v>
       </c>
       <c r="AG11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.80264449999999476</v>
       </c>
       <c r="AH11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.89590429176335284</v>
       </c>
     </row>
@@ -4297,7 +5511,7 @@
         <v>-1</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="G12">
@@ -4346,7 +5560,7 @@
         <v>214</v>
       </c>
       <c r="V12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
       <c r="W12">
@@ -4360,7 +5574,7 @@
         <v>537.67200000000003</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>518.83600000000001</v>
       </c>
       <c r="AA12">
@@ -4368,11 +5582,11 @@
         <v>709.58979200000101</v>
       </c>
       <c r="AB12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>26.638126660859637</v>
       </c>
       <c r="AC12">
-        <f>AVERAGE(L12,V12)</f>
+        <f t="shared" si="0"/>
         <v>66.5</v>
       </c>
       <c r="AD12">
@@ -4380,19 +5594,19 @@
         <v>0.5</v>
       </c>
       <c r="AE12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.70710678118654757</v>
       </c>
       <c r="AF12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>63.945300000000003</v>
       </c>
       <c r="AG12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>9.8841800000008823E-3</v>
       </c>
       <c r="AH12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>9.9419213434833023E-2</v>
       </c>
     </row>
@@ -4413,7 +5627,7 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G13">
@@ -4462,7 +5676,7 @@
         <v>182</v>
       </c>
       <c r="V13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>69</v>
       </c>
       <c r="W13">
@@ -4476,19 +5690,19 @@
         <v>342.47899999999998</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>366.23950000000002</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1129.1227205000007</v>
       </c>
       <c r="AB13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>33.602421348765937</v>
       </c>
       <c r="AC13">
-        <f>AVERAGE(L13,V13)</f>
+        <f t="shared" si="0"/>
         <v>71</v>
       </c>
       <c r="AD13">
@@ -4496,19 +5710,19 @@
         <v>8</v>
       </c>
       <c r="AE13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.8284271247461903</v>
       </c>
       <c r="AF13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>63.241250000000001</v>
       </c>
       <c r="AG13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.20640312499999891</v>
       </c>
       <c r="AH13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.45431610691235558</v>
       </c>
     </row>
@@ -4529,7 +5743,7 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="G14">
@@ -4578,7 +5792,7 @@
         <v>214</v>
       </c>
       <c r="V14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>63</v>
       </c>
       <c r="W14">
@@ -4592,39 +5806,39 @@
         <v>369.22699999999998</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>384.61349999999999</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>473.48876450000074</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>21.759796977453643</v>
       </c>
       <c r="AC14">
-        <f>AVERAGE(L14,V14)</f>
+        <f t="shared" si="0"/>
         <v>62.5</v>
       </c>
       <c r="AD14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.70710678118654757</v>
       </c>
       <c r="AF14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>65.96875</v>
       </c>
       <c r="AG14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.876953125</v>
       </c>
       <c r="AH14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.3700193885489358</v>
       </c>
     </row>
@@ -4645,7 +5859,7 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="G15">
@@ -4694,7 +5908,7 @@
         <v>200</v>
       </c>
       <c r="V15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
       <c r="W15">
@@ -4708,39 +5922,39 @@
         <v>409.827</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>434.4135</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1208.9919645</v>
       </c>
       <c r="AB15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>34.770561751286102</v>
       </c>
       <c r="AC15">
-        <f>AVERAGE(L15,V15)</f>
+        <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="AD15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="AE15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="AF15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>70.8125</v>
       </c>
       <c r="AG15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.3203125</v>
       </c>
       <c r="AH15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.1490485194281397</v>
       </c>
     </row>
@@ -4761,7 +5975,7 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G16">
@@ -4811,7 +6025,7 @@
         <v>220</v>
       </c>
       <c r="V16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="W16">
@@ -4825,39 +6039,39 @@
         <v>380.10700000000003</v>
       </c>
       <c r="Z16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>400.91899999999998</v>
       </c>
       <c r="AA16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>866.27868799999862</v>
       </c>
       <c r="AB16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>29.43261266010883</v>
       </c>
       <c r="AC16">
-        <f>AVERAGE(L16,V16)</f>
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="AD16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="AE16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.8284271247461903</v>
       </c>
       <c r="AF16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>61.545000000000002</v>
       </c>
       <c r="AG16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.59405000000000374</v>
       </c>
       <c r="AH16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.77074639149333923</v>
       </c>
     </row>

</xml_diff>